<commit_message>
fixed bug due to missing dd
</commit_message>
<xml_diff>
--- a/output_highsierra/xyz_age_eros.xlsx
+++ b/output_highsierra/xyz_age_eros.xlsx
@@ -441,7 +441,7 @@
         <v>20.30210208814082</v>
       </c>
       <c r="E2">
-        <v>3.814858059989859</v>
+        <v>3.78300140314787</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -467,7 +467,7 @@
         <v>21.15177014312552</v>
       </c>
       <c r="E3">
-        <v>3.676936155363612</v>
+        <v>3.649849202651979</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -493,7 +493,7 @@
         <v>20.80731012083443</v>
       </c>
       <c r="E4">
-        <v>3.753559435711527</v>
+        <v>3.723822647371918</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -519,7 +519,7 @@
         <v>20.5776701059737</v>
       </c>
       <c r="E5">
-        <v>3.804641622610137</v>
+        <v>3.773138277185212</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -545,7 +545,7 @@
         <v>22.75925024715065</v>
       </c>
       <c r="E6">
-        <v>3.319360847073344</v>
+        <v>3.304639793958926</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -571,7 +571,7 @@
         <v>22.4607182278317</v>
       </c>
       <c r="E7">
-        <v>3.385767690041536</v>
+        <v>3.368750112716207</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -597,7 +597,7 @@
         <v>21.88661819067987</v>
       </c>
       <c r="E8">
-        <v>3.513473157288061</v>
+        <v>3.492039187249441</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -623,7 +623,7 @@
         <v>24.435622355634</v>
       </c>
       <c r="E9">
-        <v>2.946460882713492</v>
+        <v>2.944635696321886</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -649,7 +649,7 @@
         <v>23.86152231848217</v>
       </c>
       <c r="E10">
-        <v>3.074166349960016</v>
+        <v>3.067924770855119</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -675,7 +675,7 @@
         <v>23.54002629767714</v>
       </c>
       <c r="E11">
-        <v>3.14568141161807</v>
+        <v>3.136966652593729</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>22.4607182278317</v>
       </c>
       <c r="E12">
-        <v>3.385767690041536</v>
+        <v>3.368750112716207</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -727,7 +727,7 @@
         <v>25.79049844331232</v>
       </c>
       <c r="E13">
-        <v>2.645075980011693</v>
+        <v>2.653673480423457</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -753,7 +753,7 @@
         <v>26.41052648343629</v>
       </c>
       <c r="E14">
-        <v>2.507154075385447</v>
+        <v>2.520521279927565</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -779,7 +779,7 @@
         <v>26.20385047006163</v>
       </c>
       <c r="E15">
-        <v>2.553128043594196</v>
+        <v>2.564905346759529</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -805,7 +805,7 @@
         <v>24.7800823779251</v>
       </c>
       <c r="E16">
-        <v>2.869837602365577</v>
+        <v>2.870662251601947</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -831,7 +831,7 @@
         <v>23.70077430807965</v>
       </c>
       <c r="E17">
-        <v>3.109923880789043</v>
+        <v>3.102445711724425</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -857,7 +857,7 @@
         <v>22.27700621594312</v>
       </c>
       <c r="E18">
-        <v>3.426633439560424</v>
+        <v>3.408202616566842</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -883,7 +883,7 @@
         <v>27.03055452356027</v>
       </c>
       <c r="E19">
-        <v>2.3692321707592</v>
+        <v>2.387369079431673</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -909,7 +909,7 @@
         <v>27.12241052950456</v>
       </c>
       <c r="E20">
-        <v>2.348799295999756</v>
+        <v>2.367642827506356</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -935,7 +935,7 @@
         <v>27.12241052950456</v>
       </c>
       <c r="E21">
-        <v>2.348799295999756</v>
+        <v>2.367642827506356</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -961,7 +961,7 @@
         <v>26.41052648343629</v>
       </c>
       <c r="E22">
-        <v>2.507154075385447</v>
+        <v>2.520521279927565</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -987,7 +987,7 @@
         <v>24.71119037346688</v>
       </c>
       <c r="E23">
-        <v>2.88516225843516</v>
+        <v>2.885456940545934</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>23.7467023110518</v>
       </c>
       <c r="E24">
-        <v>3.099707443409321</v>
+        <v>3.092582585761766</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1039,7 +1039,7 @@
         <v>22.43775422634562</v>
       </c>
       <c r="E25">
-        <v>3.390875908731397</v>
+        <v>3.373681675697537</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1065,7 +1065,7 @@
         <v>28.04097058894749</v>
       </c>
       <c r="E26">
-        <v>2.144470548405317</v>
+        <v>2.170380308253184</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1091,7 +1091,7 @@
         <v>28.01800658746141</v>
       </c>
       <c r="E27">
-        <v>2.149578767095178</v>
+        <v>2.175311871234513</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1117,7 +1117,7 @@
         <v>27.85725857705891</v>
       </c>
       <c r="E28">
-        <v>2.185336297924205</v>
+        <v>2.209832812103818</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1143,7 +1143,7 @@
         <v>27.30612254139315</v>
       </c>
       <c r="E29">
-        <v>2.307933546480869</v>
+        <v>2.328190323655722</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1169,7 +1169,7 @@
         <v>25.88235444925661</v>
       </c>
       <c r="E30">
-        <v>2.624643105252249</v>
+        <v>2.633947228498139</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1195,7 +1195,7 @@
         <v>24.55044236306436</v>
       </c>
       <c r="E31">
-        <v>2.920919789264186</v>
+        <v>2.91997788141524</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1221,7 +1221,7 @@
         <v>23.79263031402395</v>
       </c>
       <c r="E32">
-        <v>3.089491006029599</v>
+        <v>3.082719459799107</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1247,7 +1247,7 @@
         <v>23.21853027687212</v>
       </c>
       <c r="E33">
-        <v>3.217196473276124</v>
+        <v>3.20600853433234</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1273,7 +1273,7 @@
         <v>29.55659468702832</v>
       </c>
       <c r="E34">
-        <v>2.287163824586539</v>
+        <v>2.201243596058931</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1299,7 +1299,7 @@
         <v>29.21213466473723</v>
       </c>
       <c r="E35">
-        <v>2.327792381219808</v>
+        <v>2.236995833493242</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1325,7 +1325,7 @@
         <v>28.59210662461325</v>
       </c>
       <c r="E36">
-        <v>2.400923783159693</v>
+        <v>2.301349860875002</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1351,7 +1351,7 @@
         <v>27.76540257111461</v>
       </c>
       <c r="E37">
-        <v>2.205769172683649</v>
+        <v>2.229559064029135</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -1377,7 +1377,7 @@
         <v>26.0660664611452</v>
       </c>
       <c r="E38">
-        <v>2.583777355733361</v>
+        <v>2.594494724647505</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1403,7 +1403,7 @@
         <v>24.87193838386938</v>
       </c>
       <c r="E39">
-        <v>2.849404727606133</v>
+        <v>2.850935999676629</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1429,7 +1429,7 @@
         <v>23.72373830956573</v>
       </c>
       <c r="E40">
-        <v>3.104815662099182</v>
+        <v>3.097514148743095</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1455,7 +1455,7 @@
         <v>23.93041432294039</v>
       </c>
       <c r="E41">
-        <v>3.058841693890433</v>
+        <v>3.053130081911131</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1481,7 +1481,7 @@
         <v>24.52747836157829</v>
       </c>
       <c r="E42">
-        <v>2.926028007954048</v>
+        <v>2.924909444396569</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1507,7 +1507,7 @@
         <v>31.34778680294203</v>
       </c>
       <c r="E43">
-        <v>2.075895330093538</v>
+        <v>2.015331961400515</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -1533,7 +1533,7 @@
         <v>30.7736867657902</v>
       </c>
       <c r="E44">
-        <v>2.143609591148987</v>
+        <v>2.074919023791033</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -1559,7 +1559,7 @@
         <v>29.87809070783335</v>
       </c>
       <c r="E45">
-        <v>2.249243838395487</v>
+        <v>2.167874841120241</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -1585,7 +1585,7 @@
         <v>28.22468260083608</v>
       </c>
       <c r="E46">
-        <v>2.44426091023518</v>
+        <v>2.339485580804933</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -1611,7 +1611,7 @@
         <v>27.19130253396278</v>
       </c>
       <c r="E47">
-        <v>2.333474639930174</v>
+        <v>2.352848138562368</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -1637,7 +1637,7 @@
         <v>25.51493042547943</v>
       </c>
       <c r="E48">
-        <v>2.706374604290025</v>
+        <v>2.712852236199408</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -1663,7 +1663,7 @@
         <v>24.38969435266185</v>
       </c>
       <c r="E49">
-        <v>2.956677320093213</v>
+        <v>2.954498822284545</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -1689,7 +1689,7 @@
         <v>24.52747836157829</v>
       </c>
       <c r="E50">
-        <v>2.926028007954048</v>
+        <v>2.924909444396569</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -1715,7 +1715,7 @@
         <v>24.9408303883276</v>
       </c>
       <c r="E51">
-        <v>2.83408007153655</v>
+        <v>2.836141310732641</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -1741,7 +1741,7 @@
         <v>25.83642644628446</v>
       </c>
       <c r="E52">
-        <v>2.634859542631971</v>
+        <v>2.643810354460798</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -1767,7 +1767,7 @@
         <v>33.48343894114684</v>
       </c>
       <c r="E53">
-        <v>1.823998278967268</v>
+        <v>1.793668089307787</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -1793,7 +1793,7 @@
         <v>32.70266289062035</v>
       </c>
       <c r="E54">
-        <v>1.916089674002679</v>
+        <v>1.874706494158892</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -1819,7 +1819,7 @@
         <v>31.78410283117743</v>
       </c>
       <c r="E55">
-        <v>2.024432491691397</v>
+        <v>1.970045793983721</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -1845,7 +1845,7 @@
         <v>31.48557081185847</v>
       </c>
       <c r="E56">
-        <v>2.05964390744023</v>
+        <v>2.00103106642679</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -1871,7 +1871,7 @@
         <v>30.06180271972193</v>
       </c>
       <c r="E57">
-        <v>2.227575274857744</v>
+        <v>2.148806981155275</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -1897,7 +1897,7 @@
         <v>28.6380346275854</v>
       </c>
       <c r="E58">
-        <v>2.395506642275257</v>
+        <v>2.29658289588376</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -1923,7 +1923,7 @@
         <v>27.23723053693493</v>
       </c>
       <c r="E59">
-        <v>2.323258202550451</v>
+        <v>2.342985012599709</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -1949,7 +1949,7 @@
         <v>25.58382242993765</v>
       </c>
       <c r="E60">
-        <v>2.691049948220442</v>
+        <v>2.69805754725542</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -1975,7 +1975,7 @@
         <v>25.05565039575797</v>
       </c>
       <c r="E61">
-        <v>2.808538978087245</v>
+        <v>2.811483495825994</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2001,7 +2001,7 @@
         <v>25.44603842102122</v>
       </c>
       <c r="E62">
-        <v>2.721699260359608</v>
+        <v>2.727646925143397</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2027,7 +2027,7 @@
         <v>25.85939044777054</v>
       </c>
       <c r="E63">
-        <v>2.62975132394211</v>
+        <v>2.638878791479469</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2053,7 +2053,7 @@
         <v>35.66501908232379</v>
       </c>
       <c r="E64">
-        <v>1.566684086956562</v>
+        <v>1.567237252223818</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2079,7 +2079,7 @@
         <v>34.65460301693658</v>
       </c>
       <c r="E65">
-        <v>1.685861186414153</v>
+        <v>1.67211048203113</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2105,7 +2105,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E66">
-        <v>1.878169687811627</v>
+        <v>1.841337739220201</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2131,7 +2131,7 @@
         <v>32.24338286089889</v>
       </c>
       <c r="E67">
-        <v>1.970261082847038</v>
+        <v>1.922376144071306</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2157,7 +2157,7 @@
         <v>31.18703879253952</v>
       </c>
       <c r="E68">
-        <v>2.094855323189064</v>
+        <v>2.03201633886986</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2183,7 +2183,7 @@
         <v>30.15365872566623</v>
       </c>
       <c r="E69">
-        <v>2.216740993088872</v>
+        <v>2.139273051172792</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2209,7 +2209,7 @@
         <v>28.20171859935</v>
       </c>
       <c r="E70">
-        <v>2.381237906655291</v>
+        <v>2.302705588505786</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2235,7 +2235,7 @@
         <v>26.89277051464383</v>
       </c>
       <c r="E71">
-        <v>2.399881482898366</v>
+        <v>2.416958457319649</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2261,7 +2261,7 @@
         <v>25.6297504329098</v>
       </c>
       <c r="E72">
-        <v>2.680833510840721</v>
+        <v>2.688194421292762</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2287,7 +2287,7 @@
         <v>25.65271443439588</v>
       </c>
       <c r="E73">
-        <v>2.675725292150859</v>
+        <v>2.683262858311433</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -2313,7 +2313,7 @@
         <v>26.64016649829703</v>
       </c>
       <c r="E74">
-        <v>2.456071888486837</v>
+        <v>2.471205650114272</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -2339,7 +2339,7 @@
         <v>27.53576255625388</v>
       </c>
       <c r="E75">
-        <v>2.256851359582258</v>
+        <v>2.278874693842428</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -2365,7 +2365,7 @@
         <v>35.84873109421238</v>
       </c>
       <c r="E76">
-        <v>1.545015523418819</v>
+        <v>1.548169392258852</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -2391,7 +2391,7 @@
         <v>36.53765113879458</v>
       </c>
       <c r="E77">
-        <v>1.46375841015228</v>
+        <v>1.47666491739023</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -2417,7 +2417,7 @@
         <v>35.04499104219982</v>
       </c>
       <c r="E78">
-        <v>1.639815488896447</v>
+        <v>1.631591279605578</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -2443,7 +2443,7 @@
         <v>33.29972692925826</v>
       </c>
       <c r="E79">
-        <v>1.845666842505012</v>
+        <v>1.812735949272753</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -2469,7 +2469,7 @@
         <v>32.08263485049638</v>
       </c>
       <c r="E80">
-        <v>1.989221075942563</v>
+        <v>1.939060521540651</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -2495,7 +2495,7 @@
         <v>31.09518278659523</v>
       </c>
       <c r="E81">
-        <v>2.105689604957936</v>
+        <v>2.041550268852343</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -2521,7 +2521,7 @@
         <v>29.30399067068151</v>
       </c>
       <c r="E82">
-        <v>2.316958099450936</v>
+        <v>2.227461903510759</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -2547,7 +2547,7 @@
         <v>28.2935746052943</v>
       </c>
       <c r="E83">
-        <v>2.436135198908526</v>
+        <v>2.332335133318071</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -2573,7 +2573,7 @@
         <v>26.47941848789451</v>
       </c>
       <c r="E84">
-        <v>2.491829419315864</v>
+        <v>2.505726590983577</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -2599,7 +2599,7 @@
         <v>26.08903046263127</v>
       </c>
       <c r="E85">
-        <v>2.578669137043501</v>
+        <v>2.589563161666176</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -2625,7 +2625,7 @@
         <v>26.86980651315776</v>
       </c>
       <c r="E86">
-        <v>2.404989701588227</v>
+        <v>2.421890020300979</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -2651,7 +2651,7 @@
         <v>28.04097058894749</v>
       </c>
       <c r="E87">
-        <v>2.144470548405317</v>
+        <v>2.170380308253184</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -2677,7 +2677,7 @@
         <v>28.86767464244613</v>
       </c>
       <c r="E88">
-        <v>2.368420937853077</v>
+        <v>2.272748070927553</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -2703,7 +2703,7 @@
         <v>37.08878717446034</v>
       </c>
       <c r="E89">
-        <v>1.452107043916901</v>
+        <v>1.46825058720434</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -2729,7 +2729,7 @@
         <v>37.24953518486285</v>
       </c>
       <c r="E90">
-        <v>1.46709980269819</v>
+        <v>1.482613914095272</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -2755,7 +2755,7 @@
         <v>34.65460301693658</v>
       </c>
       <c r="E91">
-        <v>1.685861186414153</v>
+        <v>1.67211048203113</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -2781,7 +2781,7 @@
         <v>33.6901149545215</v>
       </c>
       <c r="E92">
-        <v>1.799621144987307</v>
+        <v>1.7722167468472</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -2807,7 +2807,7 @@
         <v>31.87595883712171</v>
       </c>
       <c r="E93">
-        <v>2.013598209922525</v>
+        <v>1.960511864001238</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -2833,7 +2833,7 @@
         <v>30.84257877024842</v>
       </c>
       <c r="E94">
-        <v>2.135483879822333</v>
+        <v>2.067768576304171</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -2859,7 +2859,7 @@
         <v>29.21213466473723</v>
       </c>
       <c r="E95">
-        <v>2.327792381219808</v>
+        <v>2.236995833493242</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>27.90318658003105</v>
       </c>
       <c r="E96">
-        <v>2.175119860544483</v>
+        <v>2.199969686141159</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -2911,7 +2911,7 @@
         <v>27.07648252653242</v>
       </c>
       <c r="E97">
-        <v>2.359015733379478</v>
+        <v>2.377505953469015</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -2937,7 +2937,7 @@
         <v>27.51279855476781</v>
       </c>
       <c r="E98">
-        <v>2.26195957827212</v>
+        <v>2.283806256823758</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -2963,7 +2963,7 @@
         <v>28.31653860678037</v>
       </c>
       <c r="E99">
-        <v>2.433426628466308</v>
+        <v>2.32995165082245</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -2989,7 +2989,7 @@
         <v>29.4877026825701</v>
       </c>
       <c r="E100">
-        <v>2.295289535913192</v>
+        <v>2.208394043545793</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3015,7 +3015,7 @@
         <v>30.56701075241554</v>
       </c>
       <c r="E101">
-        <v>2.167986725128948</v>
+        <v>2.096370366251619</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -3041,7 +3041,7 @@
         <v>38.00734723390327</v>
       </c>
       <c r="E102">
-        <v>1.537779951238552</v>
+        <v>1.550326740866808</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -3067,7 +3067,7 @@
         <v>38.4895912651108</v>
       </c>
       <c r="E103">
-        <v>1.582758227582419</v>
+        <v>1.593416721539604</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -3093,7 +3093,7 @@
         <v>37.18064318040463</v>
       </c>
       <c r="E104">
-        <v>1.460674334649066</v>
+        <v>1.476458202570587</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3119,7 +3119,7 @@
         <v>33.91975496938223</v>
       </c>
       <c r="E105">
-        <v>1.772535440565127</v>
+        <v>1.748381921890993</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3145,7 +3145,7 @@
         <v>32.93230290548109</v>
       </c>
       <c r="E106">
-        <v>1.889003969580499</v>
+        <v>1.850871669202684</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3171,7 +3171,7 @@
         <v>31.14111078956738</v>
       </c>
       <c r="E107">
-        <v>2.1002724640735</v>
+        <v>2.036783303861101</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3197,7 +3197,7 @@
         <v>29.80919870337513</v>
       </c>
       <c r="E108">
-        <v>2.257369549722141</v>
+        <v>2.175025288607103</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -3223,7 +3223,7 @@
         <v>28.45432261569681</v>
       </c>
       <c r="E109">
-        <v>2.417175205813</v>
+        <v>2.315650755848726</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -3249,7 +3249,7 @@
         <v>27.71947456814247</v>
       </c>
       <c r="E110">
-        <v>2.215985610063371</v>
+        <v>2.239422189991794</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -3275,7 +3275,7 @@
         <v>27.92615058151713</v>
       </c>
       <c r="E111">
-        <v>2.170011641854622</v>
+        <v>2.19503812315983</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -3301,7 +3301,7 @@
         <v>29.21213466473723</v>
       </c>
       <c r="E112">
-        <v>2.327792381219808</v>
+        <v>2.236995833493242</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -3327,7 +3327,7 @@
         <v>30.33737073755481</v>
       </c>
       <c r="E113">
-        <v>2.195072429551128</v>
+        <v>2.120205191207826</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -3353,7 +3353,7 @@
         <v>31.1181467880813</v>
       </c>
       <c r="E114">
-        <v>2.102981034515718</v>
+        <v>2.039166786356722</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -3379,7 +3379,7 @@
         <v>39.38518732306765</v>
       </c>
       <c r="E115">
-        <v>1.666289312221029</v>
+        <v>1.673440971360511</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -3405,7 +3405,7 @@
         <v>39.06369130226264</v>
       </c>
       <c r="E116">
-        <v>1.636303794658451</v>
+        <v>1.644714317578647</v>
       </c>
       <c r="F116">
         <v>1</v>
@@ -3431,7 +3431,7 @@
         <v>36.67543514771102</v>
       </c>
       <c r="E117">
-        <v>1.447506987498973</v>
+        <v>1.462364022416506</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -3457,7 +3457,7 @@
         <v>33.64418695154936</v>
       </c>
       <c r="E118">
-        <v>1.805038285871742</v>
+        <v>1.776983711838442</v>
       </c>
       <c r="F118">
         <v>1</v>
@@ -3483,7 +3483,7 @@
         <v>32.67969888913428</v>
       </c>
       <c r="E119">
-        <v>1.918798244444897</v>
+        <v>1.877089976654512</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -3509,7 +3509,7 @@
         <v>31.32482280145596</v>
       </c>
       <c r="E120">
-        <v>2.078603900535756</v>
+        <v>2.017715443896135</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -3535,7 +3535,7 @@
         <v>29.85512670634728</v>
       </c>
       <c r="E121">
-        <v>2.251952408837705</v>
+        <v>2.170258323615862</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -3561,7 +3561,7 @@
         <v>28.86767464244613</v>
       </c>
       <c r="E122">
-        <v>2.368420937853077</v>
+        <v>2.272748070927553</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -3587,7 +3587,7 @@
         <v>29.07435065582079</v>
       </c>
       <c r="E123">
-        <v>2.344043803873116</v>
+        <v>2.251296728466966</v>
       </c>
       <c r="F123">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         <v>29.60252269000047</v>
       </c>
       <c r="E124">
-        <v>2.281746683702103</v>
+        <v>2.19647663106769</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -3639,7 +3639,7 @@
         <v>30.7736867657902</v>
       </c>
       <c r="E125">
-        <v>2.143609591148987</v>
+        <v>2.074919023791033</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -3665,7 +3665,7 @@
         <v>31.83003083414957</v>
       </c>
       <c r="E126">
-        <v>2.019015350806961</v>
+        <v>1.965278828992479</v>
       </c>
       <c r="F126">
         <v>1</v>
@@ -3691,7 +3691,7 @@
         <v>39.95928736021949</v>
       </c>
       <c r="E127">
-        <v>1.719834879297061</v>
+        <v>1.724738567399554</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -3717,7 +3717,7 @@
         <v>40.51042339588524</v>
       </c>
       <c r="E128">
-        <v>1.71924190197483</v>
+        <v>1.72281989810854</v>
       </c>
       <c r="F128">
         <v>1</v>
@@ -3743,7 +3743,7 @@
         <v>39.04072730077657</v>
       </c>
       <c r="E129">
-        <v>1.634161971975409</v>
+        <v>1.642662413737086</v>
       </c>
       <c r="F129">
         <v>1</v>
@@ -3769,7 +3769,7 @@
         <v>35.77983908975416</v>
       </c>
       <c r="E130">
-        <v>1.553141234745473</v>
+        <v>1.555319839745714</v>
       </c>
       <c r="F130">
         <v>1</v>
@@ -3795,7 +3795,7 @@
         <v>33.80493496195187</v>
       </c>
       <c r="E131">
-        <v>1.786078292776217</v>
+        <v>1.760299334369097</v>
       </c>
       <c r="F131">
         <v>1</v>
@@ -3821,7 +3821,7 @@
         <v>32.63377088616213</v>
       </c>
       <c r="E132">
-        <v>1.924215385329333</v>
+        <v>1.881856941645754</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -3847,7 +3847,7 @@
         <v>30.72775876281806</v>
       </c>
       <c r="E133">
-        <v>2.149026732033423</v>
+        <v>2.079685988782274</v>
       </c>
       <c r="F133">
         <v>1</v>
@@ -3873,7 +3873,7 @@
         <v>29.90105470931942</v>
       </c>
       <c r="E134">
-        <v>2.246535267953269</v>
+        <v>2.16549135862462</v>
       </c>
       <c r="F134">
         <v>1</v>
@@ -3899,7 +3899,7 @@
         <v>30.03883871823586</v>
       </c>
       <c r="E135">
-        <v>2.230283845299962</v>
+        <v>2.151190463650896</v>
       </c>
       <c r="F135">
         <v>1</v>
@@ -3925,7 +3925,7 @@
         <v>30.24551473161052</v>
       </c>
       <c r="E136">
-        <v>2.20590671132</v>
+        <v>2.129739121190309</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -3951,7 +3951,7 @@
         <v>30.54404675092947</v>
       </c>
       <c r="E137">
-        <v>2.170695295571166</v>
+        <v>2.09875384874724</v>
       </c>
       <c r="F137">
         <v>1</v>
@@ -3977,7 +3977,7 @@
         <v>31.55446281631669</v>
       </c>
       <c r="E138">
-        <v>2.051518196113577</v>
+        <v>1.993880618939928</v>
       </c>
       <c r="F138">
         <v>1</v>
@@ -4003,7 +4003,7 @@
         <v>32.81748289805072</v>
       </c>
       <c r="E139">
-        <v>1.902546821791589</v>
+        <v>1.862789081680788</v>
       </c>
       <c r="F139">
         <v>1</v>
@@ -4029,7 +4029,7 @@
         <v>41.77344347761927</v>
       </c>
       <c r="E140">
-        <v>1.658303418646026</v>
+        <v>1.659797116777729</v>
       </c>
       <c r="F140">
         <v>1</v>
@@ -4055,7 +4055,7 @@
         <v>42.20975950585466</v>
       </c>
       <c r="E141">
-        <v>1.637251942586985</v>
+        <v>1.638025610499813</v>
       </c>
       <c r="F141">
         <v>1</v>
@@ -4081,7 +4081,7 @@
         <v>39.7755753483309</v>
       </c>
       <c r="E142">
-        <v>1.70270029783273</v>
+        <v>1.708323336667061</v>
       </c>
       <c r="F142">
         <v>1</v>
@@ -4107,7 +4107,7 @@
         <v>37.96141923093112</v>
       </c>
       <c r="E143">
-        <v>1.533496305872469</v>
+        <v>1.546222933183685</v>
       </c>
       <c r="F143">
         <v>1</v>
@@ -4133,7 +4133,7 @@
         <v>35.45834306894914</v>
       </c>
       <c r="E144">
-        <v>1.591061220936524</v>
+        <v>1.588688594684404</v>
       </c>
       <c r="F144">
         <v>1</v>
@@ -4159,7 +4159,7 @@
         <v>33.50640294263292</v>
       </c>
       <c r="E145">
-        <v>1.82128970852505</v>
+        <v>1.791284606812166</v>
       </c>
       <c r="F145">
         <v>1</v>
@@ -4185,7 +4185,7 @@
         <v>32.35820286832926</v>
       </c>
       <c r="E146">
-        <v>1.956718230635948</v>
+        <v>1.910458731593202</v>
       </c>
       <c r="F146">
         <v>1</v>
@@ -4211,7 +4211,7 @@
         <v>30.8655427717345</v>
       </c>
       <c r="E147">
-        <v>2.132775309380115</v>
+        <v>2.06538509380855</v>
       </c>
       <c r="F147">
         <v>1</v>
@@ -4237,7 +4237,7 @@
         <v>30.7736867657902</v>
       </c>
       <c r="E148">
-        <v>2.143609591148987</v>
+        <v>2.074919023791033</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -4263,7 +4263,7 @@
         <v>31.27889479848381</v>
       </c>
       <c r="E149">
-        <v>2.084021041420192</v>
+        <v>2.022482408887377</v>
       </c>
       <c r="F149">
         <v>1</v>
@@ -4289,7 +4289,7 @@
         <v>31.62335482077491</v>
       </c>
       <c r="E150">
-        <v>2.043392484786922</v>
+        <v>1.986730171453066</v>
       </c>
       <c r="F150">
         <v>1</v>
@@ -4315,7 +4315,7 @@
         <v>32.17449085644067</v>
       </c>
       <c r="E151">
-        <v>1.978386794173692</v>
+        <v>1.929526591558168</v>
       </c>
       <c r="F151">
         <v>1</v>
@@ -4341,7 +4341,7 @@
         <v>33.07008691439753</v>
       </c>
       <c r="E152">
-        <v>1.872752546927191</v>
+        <v>1.83657077422896</v>
       </c>
       <c r="F152">
         <v>1</v>
@@ -4367,7 +4367,7 @@
         <v>33.87382696641009</v>
       </c>
       <c r="E153">
-        <v>1.777952581449563</v>
+        <v>1.753148886882235</v>
       </c>
       <c r="F153">
         <v>1</v>
@@ -4393,7 +4393,7 @@
         <v>43.31203157718618</v>
       </c>
       <c r="E154">
-        <v>1.584069266227302</v>
+        <v>1.583023910429287</v>
       </c>
       <c r="F154">
         <v>1</v>
@@ -4419,7 +4419,7 @@
         <v>42.18679550436859</v>
       </c>
       <c r="E155">
-        <v>1.638359915011145</v>
+        <v>1.639171479251282</v>
       </c>
       <c r="F155">
         <v>1</v>
@@ -4445,7 +4445,7 @@
         <v>39.08665530374871</v>
       </c>
       <c r="E156">
-        <v>1.638445617341492</v>
+        <v>1.646766221420209</v>
       </c>
       <c r="F156">
         <v>1</v>
@@ -4471,7 +4471,7 @@
         <v>37.36435519229322</v>
       </c>
       <c r="E157">
-        <v>1.477808916113396</v>
+        <v>1.49287343330308</v>
       </c>
       <c r="F157">
         <v>1</v>
@@ -4497,7 +4497,7 @@
         <v>34.86127903031124</v>
       </c>
       <c r="E158">
-        <v>1.661484052434191</v>
+        <v>1.650659139570543</v>
       </c>
       <c r="F158">
         <v>1</v>
@@ -4523,7 +4523,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E159">
-        <v>1.878169687811627</v>
+        <v>1.841337739220201</v>
       </c>
       <c r="F159">
         <v>1</v>
@@ -4549,7 +4549,7 @@
         <v>32.26634686238496</v>
       </c>
       <c r="E160">
-        <v>1.96755251240482</v>
+        <v>1.919992661575685</v>
       </c>
       <c r="F160">
         <v>1</v>
@@ -4575,7 +4575,7 @@
         <v>31.50853481334455</v>
       </c>
       <c r="E161">
-        <v>2.056935336998012</v>
+        <v>1.998647583931169</v>
       </c>
       <c r="F161">
         <v>1</v>
@@ -4601,7 +4601,7 @@
         <v>31.85299483563564</v>
       </c>
       <c r="E162">
-        <v>2.016306780364743</v>
+        <v>1.962895346496859</v>
       </c>
       <c r="F162">
         <v>1</v>
@@ -4627,7 +4627,7 @@
         <v>32.49598687724569</v>
       </c>
       <c r="E163">
-        <v>1.94046680798264</v>
+        <v>1.896157836619478</v>
       </c>
       <c r="F163">
         <v>1</v>
@@ -4653,7 +4653,7 @@
         <v>33.07008691439753</v>
       </c>
       <c r="E164">
-        <v>1.872752546927191</v>
+        <v>1.83657077422896</v>
       </c>
       <c r="F164">
         <v>1</v>
@@ -4679,7 +4679,7 @@
         <v>33.85086296492401</v>
       </c>
       <c r="E165">
-        <v>1.780661151891781</v>
+        <v>1.755532369377855</v>
       </c>
       <c r="F165">
         <v>1</v>
@@ -4705,7 +4705,7 @@
         <v>34.33310699613155</v>
       </c>
       <c r="E166">
-        <v>1.723781172605204</v>
+        <v>1.70547923696982</v>
       </c>
       <c r="F166">
         <v>1</v>
@@ -4731,7 +4731,7 @@
         <v>43.2890675757001</v>
       </c>
       <c r="E167">
-        <v>1.585177238651462</v>
+        <v>1.584169779180757</v>
       </c>
       <c r="F167">
         <v>1</v>
@@ -4757,7 +4757,7 @@
         <v>43.90909561582409</v>
       </c>
       <c r="E168">
-        <v>1.55526198319914</v>
+        <v>1.553231322891086</v>
       </c>
       <c r="F168">
         <v>1</v>
@@ -4783,7 +4783,7 @@
         <v>42.82978754597865</v>
       </c>
       <c r="E169">
-        <v>1.607336687134663</v>
+        <v>1.607087154210142</v>
       </c>
       <c r="F169">
         <v>1</v>
@@ -4809,7 +4809,7 @@
         <v>38.09920323984756</v>
       </c>
       <c r="E170">
-        <v>1.546347241970717</v>
+        <v>1.558534356233055</v>
       </c>
       <c r="F170">
         <v>1</v>
@@ -4835,7 +4835,7 @@
         <v>36.90507516257176</v>
       </c>
       <c r="E171">
-        <v>1.434972462452571</v>
+        <v>1.451835356471846</v>
       </c>
       <c r="F171">
         <v>1</v>
@@ -4861,7 +4861,7 @@
         <v>34.28717899315941</v>
       </c>
       <c r="E172">
-        <v>1.72919831348964</v>
+        <v>1.710246201961061</v>
       </c>
       <c r="F172">
         <v>1</v>
@@ -4887,7 +4887,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E173">
-        <v>1.878169687811627</v>
+        <v>1.841337739220201</v>
       </c>
       <c r="F173">
         <v>1</v>
@@ -4913,7 +4913,7 @@
         <v>32.88637490250894</v>
       </c>
       <c r="E174">
-        <v>1.894421110464935</v>
+        <v>1.855638634193926</v>
       </c>
       <c r="F174">
         <v>1</v>
@@ -4939,7 +4939,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E175">
-        <v>1.878169687811627</v>
+        <v>1.841337739220201</v>
       </c>
       <c r="F175">
         <v>1</v>
@@ -4965,7 +4965,7 @@
         <v>33.48343894114684</v>
       </c>
       <c r="E176">
-        <v>1.823998278967268</v>
+        <v>1.793668089307787</v>
       </c>
       <c r="F176">
         <v>1</v>
@@ -4991,7 +4991,7 @@
         <v>34.0345749768126</v>
       </c>
       <c r="E177">
-        <v>1.758992588354037</v>
+        <v>1.736464509412889</v>
       </c>
       <c r="F177">
         <v>1</v>
@@ -5017,7 +5017,7 @@
         <v>34.6316390154505</v>
       </c>
       <c r="E178">
-        <v>1.68856975685637</v>
+        <v>1.67449396452675</v>
       </c>
       <c r="F178">
         <v>1</v>
@@ -5043,7 +5043,7 @@
         <v>44.46023165148983</v>
       </c>
       <c r="E179">
-        <v>1.528670645019298</v>
+        <v>1.525730472855823</v>
       </c>
       <c r="F179">
         <v>1</v>
@@ -5069,7 +5069,7 @@
         <v>45.14915169607204</v>
       </c>
       <c r="E180">
-        <v>1.495431472294496</v>
+        <v>1.491354410311745</v>
       </c>
       <c r="F180">
         <v>1</v>
@@ -5095,7 +5095,7 @@
         <v>43.7253836039355</v>
       </c>
       <c r="E181">
-        <v>1.564125762592421</v>
+        <v>1.56239827290284</v>
       </c>
       <c r="F181">
         <v>1</v>
@@ -5121,7 +5121,7 @@
         <v>42.04901149545215</v>
       </c>
       <c r="E182">
-        <v>1.645007749556105</v>
+        <v>1.646046691760098</v>
       </c>
       <c r="F182">
         <v>1</v>
@@ -5147,7 +5147,7 @@
         <v>38.14513124281971</v>
       </c>
       <c r="E183">
-        <v>1.5506308873368</v>
+        <v>1.562638163916179</v>
       </c>
       <c r="F183">
         <v>1</v>
@@ -5173,7 +5173,7 @@
         <v>36.44579513285029</v>
       </c>
       <c r="E184">
-        <v>1.474592691921152</v>
+        <v>1.486198847372713</v>
       </c>
       <c r="F184">
         <v>1</v>
@@ -5199,7 +5199,7 @@
         <v>34.76942302436694</v>
       </c>
       <c r="E185">
-        <v>1.672318334203063</v>
+        <v>1.660193069553026</v>
       </c>
       <c r="F185">
         <v>1</v>
@@ -5225,7 +5225,7 @@
         <v>33.41454693668862</v>
       </c>
       <c r="E186">
-        <v>1.832123990293922</v>
+        <v>1.800818536794649</v>
       </c>
       <c r="F186">
         <v>1</v>
@@ -5251,7 +5251,7 @@
         <v>33.57529494709114</v>
       </c>
       <c r="E187">
-        <v>1.813163997198396</v>
+        <v>1.784134159325304</v>
       </c>
       <c r="F187">
         <v>1</v>
@@ -5277,7 +5277,7 @@
         <v>34.24125099018726</v>
       </c>
       <c r="E188">
-        <v>1.734615454374076</v>
+        <v>1.715013166952303</v>
       </c>
       <c r="F188">
         <v>1</v>
@@ -5303,7 +5303,7 @@
         <v>34.99906303922768</v>
       </c>
       <c r="E189">
-        <v>1.645232629780883</v>
+        <v>1.636358244596819</v>
       </c>
       <c r="F189">
         <v>1</v>
@@ -5329,7 +5329,7 @@
         <v>35.68798308380987</v>
       </c>
       <c r="E190">
-        <v>1.563975516514345</v>
+        <v>1.564853769728197</v>
       </c>
       <c r="F190">
         <v>1</v>
@@ -5355,7 +5355,7 @@
         <v>45.44768371539099</v>
       </c>
       <c r="E191">
-        <v>1.481027830780415</v>
+        <v>1.476458116542644</v>
       </c>
       <c r="F191">
         <v>1</v>
@@ -5381,7 +5381,7 @@
         <v>45.44768371539099</v>
       </c>
       <c r="E192">
-        <v>1.481027830780415</v>
+        <v>1.476458116542644</v>
       </c>
       <c r="F192">
         <v>1</v>
@@ -5407,7 +5407,7 @@
         <v>43.33499557867225</v>
       </c>
       <c r="E193">
-        <v>1.582961293803142</v>
+        <v>1.581878041677818</v>
       </c>
       <c r="F193">
         <v>1</v>
@@ -5433,7 +5433,7 @@
         <v>41.33712744938389</v>
       </c>
       <c r="E194">
-        <v>1.679354894705067</v>
+        <v>1.681568623055645</v>
       </c>
       <c r="F194">
         <v>1</v>
@@ -5459,7 +5459,7 @@
         <v>39.08665530374871</v>
       </c>
       <c r="E195">
-        <v>1.638445617341492</v>
+        <v>1.646766221420209</v>
       </c>
       <c r="F195">
         <v>1</v>
@@ -5485,7 +5485,7 @@
         <v>37.57103120566787</v>
       </c>
       <c r="E196">
-        <v>1.497085320260768</v>
+        <v>1.511340567877136</v>
       </c>
       <c r="F196">
         <v>1</v>
@@ -5511,7 +5511,7 @@
         <v>35.55019907489343</v>
       </c>
       <c r="E197">
-        <v>1.580226939167652</v>
+        <v>1.579154664701921</v>
       </c>
       <c r="F197">
         <v>1</v>
@@ -5537,7 +5537,7 @@
         <v>34.31014299464548</v>
       </c>
       <c r="E198">
-        <v>1.726489743047422</v>
+        <v>1.707862719465441</v>
       </c>
       <c r="F198">
         <v>1</v>
@@ -5563,7 +5563,7 @@
         <v>34.33310699613155</v>
       </c>
       <c r="E199">
-        <v>1.723781172605204</v>
+        <v>1.70547923696982</v>
       </c>
       <c r="F199">
         <v>1</v>
@@ -5589,7 +5589,7 @@
         <v>35.73391108678202</v>
       </c>
       <c r="E200">
-        <v>1.558558375629909</v>
+        <v>1.560086804736956</v>
       </c>
       <c r="F200">
         <v>1</v>
@@ -5615,7 +5615,7 @@
         <v>36.76729115365531</v>
       </c>
       <c r="E201">
-        <v>1.436672705730101</v>
+        <v>1.452830092434023</v>
       </c>
       <c r="F201">
         <v>1</v>
@@ -5641,7 +5641,7 @@
         <v>45.88399974362638</v>
       </c>
       <c r="E202">
-        <v>1.448989871215566</v>
+        <v>1.446053877613458</v>
       </c>
       <c r="F202">
         <v>1</v>
@@ -5667,7 +5667,7 @@
         <v>44.5750516589202</v>
       </c>
       <c r="E203">
-        <v>1.523130782898498</v>
+        <v>1.520001129098477</v>
       </c>
       <c r="F203">
         <v>1</v>
@@ -5693,7 +5693,7 @@
         <v>42.53125552665969</v>
       </c>
       <c r="E204">
-        <v>1.621740328648744</v>
+        <v>1.621983447979243</v>
       </c>
       <c r="F204">
         <v>1</v>
@@ -5719,7 +5719,7 @@
         <v>41.22230744195352</v>
       </c>
       <c r="E205">
-        <v>1.684894756825868</v>
+        <v>1.687297966812992</v>
       </c>
       <c r="F205">
         <v>1</v>
@@ -5745,7 +5745,7 @@
         <v>39.24740331415121</v>
       </c>
       <c r="E206">
-        <v>1.653438376122781</v>
+        <v>1.661129548311141</v>
       </c>
       <c r="F206">
         <v>1</v>
@@ -5771,7 +5771,7 @@
         <v>38.12216724133363</v>
       </c>
       <c r="E207">
-        <v>1.548489064653758</v>
+        <v>1.560586260074617</v>
       </c>
       <c r="F207">
         <v>1</v>
@@ -5797,7 +5797,7 @@
         <v>36.90507516257176</v>
       </c>
       <c r="E208">
-        <v>1.434972462452571</v>
+        <v>1.451835356471846</v>
       </c>
       <c r="F208">
         <v>1</v>
@@ -5823,7 +5823,7 @@
         <v>35.38945106449092</v>
       </c>
       <c r="E209">
-        <v>1.599186932263178</v>
+        <v>1.595839042171267</v>
       </c>
       <c r="F209">
         <v>1</v>
@@ -5849,7 +5849,7 @@
         <v>35.38945106449092</v>
       </c>
       <c r="E210">
-        <v>1.599186932263178</v>
+        <v>1.595839042171267</v>
       </c>
       <c r="F210">
         <v>1</v>
@@ -5875,7 +5875,7 @@
         <v>36.9510031655439</v>
       </c>
       <c r="E211">
-        <v>1.439256107818653</v>
+        <v>1.455939164154969</v>
       </c>
       <c r="F211">
         <v>1</v>
@@ -5901,7 +5901,7 @@
         <v>38.5814472710551</v>
       </c>
       <c r="E212">
-        <v>1.591325518314584</v>
+        <v>1.601624336905851</v>
       </c>
       <c r="F212">
         <v>1</v>
@@ -5927,7 +5927,7 @@
         <v>45.67732373025171</v>
       </c>
       <c r="E213">
-        <v>1.469948106538815</v>
+        <v>1.464999429027951</v>
       </c>
       <c r="F213">
         <v>1</v>
@@ -5953,7 +5953,7 @@
         <v>45.76917973619601</v>
       </c>
       <c r="E214">
-        <v>1.465516216842174</v>
+        <v>1.460415954022074</v>
       </c>
       <c r="F214">
         <v>1</v>
@@ -5979,7 +5979,7 @@
         <v>44.46023165148983</v>
       </c>
       <c r="E215">
-        <v>1.528670645019298</v>
+        <v>1.525730472855823</v>
       </c>
       <c r="F215">
         <v>1</v>
@@ -6005,7 +6005,7 @@
         <v>42.3475435147711</v>
       </c>
       <c r="E216">
-        <v>1.630604108042024</v>
+        <v>1.631150397990997</v>
       </c>
       <c r="F216">
         <v>1</v>
@@ -6031,7 +6031,7 @@
         <v>41.19934344046744</v>
       </c>
       <c r="E217">
-        <v>1.686002729250028</v>
+        <v>1.688443835564461</v>
       </c>
       <c r="F217">
         <v>1</v>
@@ -6057,7 +6057,7 @@
         <v>39.54593533347017</v>
       </c>
       <c r="E218">
-        <v>1.681282071002318</v>
+        <v>1.687804298251444</v>
       </c>
       <c r="F218">
         <v>1</v>
@@ -6083,7 +6083,7 @@
         <v>38.55848326956902</v>
       </c>
       <c r="E219">
-        <v>1.589183695631543</v>
+        <v>1.59957243306429</v>
       </c>
       <c r="F219">
         <v>1</v>
@@ -6109,7 +6109,7 @@
         <v>36.92803916405782</v>
       </c>
       <c r="E220">
-        <v>1.437114285135612</v>
+        <v>1.453887260313408</v>
       </c>
       <c r="F220">
         <v>1</v>
@@ -6135,7 +6135,7 @@
         <v>36.33097512541992</v>
       </c>
       <c r="E221">
-        <v>1.488135544132242</v>
+        <v>1.498116259850817</v>
       </c>
       <c r="F221">
         <v>1</v>
@@ -6161,7 +6161,7 @@
         <v>36.65247114622495</v>
       </c>
       <c r="E222">
-        <v>1.45021555794119</v>
+        <v>1.464747504912127</v>
       </c>
       <c r="F222">
         <v>1</v>
@@ -6187,7 +6187,7 @@
         <v>38.76515928294369</v>
       </c>
       <c r="E223">
-        <v>1.608460099778914</v>
+        <v>1.618039567638345</v>
       </c>
       <c r="F223">
         <v>1</v>
@@ -6213,7 +6213,7 @@
         <v>40.00521536319164</v>
       </c>
       <c r="E224">
-        <v>1.724118524663143</v>
+        <v>1.728842375082678</v>
       </c>
       <c r="F224">
         <v>1</v>
@@ -6239,7 +6239,7 @@
         <v>45.33286370796063</v>
       </c>
       <c r="E225">
-        <v>1.486567692901216</v>
+        <v>1.48218746029999</v>
       </c>
       <c r="F225">
         <v>1</v>
@@ -6265,7 +6265,7 @@
         <v>46.48106378226429</v>
       </c>
       <c r="E226">
-        <v>1.134534017036395</v>
+        <v>1.191810241142256</v>
       </c>
       <c r="F226">
         <v>1</v>
@@ -6291,7 +6291,7 @@
         <v>45.65435972876564</v>
       </c>
       <c r="E227">
-        <v>1.471056078962975</v>
+        <v>1.46614529777942</v>
       </c>
       <c r="F227">
         <v>1</v>
@@ -6317,7 +6317,7 @@
         <v>44.34541164405947</v>
       </c>
       <c r="E228">
-        <v>1.534210507140099</v>
+        <v>1.531459816613169</v>
       </c>
       <c r="F228">
         <v>1</v>
@@ -6343,7 +6343,7 @@
         <v>42.27865151031288</v>
       </c>
       <c r="E229">
-        <v>1.633928025314505</v>
+        <v>1.634588004245405</v>
       </c>
       <c r="F229">
         <v>1</v>
@@ -6369,7 +6369,7 @@
         <v>41.63565946870284</v>
       </c>
       <c r="E230">
-        <v>1.664951253190986</v>
+        <v>1.666672329286545</v>
       </c>
       <c r="F230">
         <v>1</v>
@@ -6395,7 +6395,7 @@
         <v>39.56889933495624</v>
       </c>
       <c r="E231">
-        <v>1.683423893685359</v>
+        <v>1.689856202093005</v>
       </c>
       <c r="F231">
         <v>1</v>
@@ -6421,7 +6421,7 @@
         <v>38.65033927551332</v>
       </c>
       <c r="E232">
-        <v>1.597750986363708</v>
+        <v>1.607780048430536</v>
       </c>
       <c r="F232">
         <v>1</v>
@@ -6447,7 +6447,7 @@
         <v>37.04285917148819</v>
       </c>
       <c r="E233">
-        <v>1.447823398550818</v>
+        <v>1.464146779521216</v>
       </c>
       <c r="F233">
         <v>1</v>
@@ -6473,7 +6473,7 @@
         <v>37.08878717446034</v>
       </c>
       <c r="E234">
-        <v>1.452107043916901</v>
+        <v>1.46825058720434</v>
       </c>
       <c r="F234">
         <v>1</v>
@@ -6499,7 +6499,7 @@
         <v>37.70881521458431</v>
       </c>
       <c r="E235">
-        <v>1.509936256359015</v>
+        <v>1.523651990926506</v>
       </c>
       <c r="F235">
         <v>1</v>
@@ -6525,7 +6525,7 @@
         <v>39.24740331415121</v>
       </c>
       <c r="E236">
-        <v>1.653438376122781</v>
+        <v>1.661129548311141</v>
       </c>
       <c r="F236">
         <v>1</v>
@@ -6551,7 +6551,7 @@
         <v>40.23485537805237</v>
       </c>
       <c r="E237">
-        <v>1.732537571064751</v>
+        <v>1.736570323126171</v>
       </c>
       <c r="F237">
         <v>1</v>
@@ -6577,7 +6577,7 @@
         <v>46.66477579415287</v>
       </c>
       <c r="E238">
-        <v>1.139243769568774</v>
+        <v>1.196410853685324</v>
       </c>
       <c r="F238">
         <v>1</v>
@@ -6603,7 +6603,7 @@
         <v>46.6418117926668</v>
       </c>
       <c r="E239">
-        <v>1.138655050502227</v>
+        <v>1.19583577711744</v>
       </c>
       <c r="F239">
         <v>1</v>
@@ -6629,7 +6629,7 @@
         <v>48.01965188183119</v>
       </c>
       <c r="E240">
-        <v>1.173978194495068</v>
+        <v>1.23034037119045</v>
       </c>
       <c r="F240">
         <v>1</v>
@@ -6655,7 +6655,7 @@
         <v>47.65222785805402</v>
       </c>
       <c r="E241">
-        <v>1.16455868943031</v>
+        <v>1.221139146104314</v>
       </c>
       <c r="F241">
         <v>1</v>
@@ -6681,7 +6681,7 @@
         <v>45.90696374511245</v>
       </c>
       <c r="E242">
-        <v>1.436895415285598</v>
+        <v>1.43627527621072</v>
       </c>
       <c r="F242">
         <v>1</v>
@@ -6707,7 +6707,7 @@
         <v>44.71283566783664</v>
       </c>
       <c r="E243">
-        <v>1.516482948353538</v>
+        <v>1.513125916589661</v>
       </c>
       <c r="F243">
         <v>1</v>
@@ -6733,7 +6733,7 @@
         <v>42.41643551922932</v>
       </c>
       <c r="E244">
-        <v>1.627280190769544</v>
+        <v>1.627712791736589</v>
       </c>
       <c r="F244">
         <v>1</v>
@@ -6759,7 +6759,7 @@
         <v>42.0949394984243</v>
       </c>
       <c r="E245">
-        <v>1.642791804707785</v>
+        <v>1.643754954257159</v>
       </c>
       <c r="F245">
         <v>1</v>
@@ -6785,7 +6785,7 @@
         <v>39.56889933495624</v>
       </c>
       <c r="E246">
-        <v>1.683423893685359</v>
+        <v>1.689856202093005</v>
       </c>
       <c r="F246">
         <v>1</v>
@@ -6811,7 +6811,7 @@
         <v>38.62737527402724</v>
       </c>
       <c r="E247">
-        <v>1.595609163680666</v>
+        <v>1.605728144588975</v>
       </c>
       <c r="F247">
         <v>1</v>
@@ -6837,7 +6837,7 @@
         <v>38.25995125025007</v>
       </c>
       <c r="E248">
-        <v>1.561340000752006</v>
+        <v>1.572897683123987</v>
       </c>
       <c r="F248">
         <v>1</v>
@@ -6863,7 +6863,7 @@
         <v>38.92590729334619</v>
       </c>
       <c r="E249">
-        <v>1.623452858560203</v>
+        <v>1.632402894529277</v>
       </c>
       <c r="F249">
         <v>1</v>
@@ -6889,7 +6889,7 @@
         <v>39.24740331415121</v>
       </c>
       <c r="E250">
-        <v>1.653438376122781</v>
+        <v>1.661129548311141</v>
       </c>
       <c r="F250">
         <v>1</v>
@@ -6915,7 +6915,7 @@
         <v>40.39560338845489</v>
       </c>
       <c r="E251">
-        <v>1.72478176409563</v>
+        <v>1.728549241865886</v>
       </c>
       <c r="F251">
         <v>1</v>
@@ -6941,7 +6941,7 @@
         <v>48.4330039085805</v>
       </c>
       <c r="E252">
-        <v>1.18457513769292</v>
+        <v>1.240691749412353</v>
       </c>
       <c r="F252">
         <v>1</v>
@@ -6967,7 +6967,7 @@
         <v>48.82339193384375</v>
       </c>
       <c r="E253">
-        <v>1.194583361824225</v>
+        <v>1.250468051066373</v>
       </c>
       <c r="F253">
         <v>1</v>
@@ -6993,7 +6993,7 @@
         <v>48.47893191155265</v>
       </c>
       <c r="E254">
-        <v>1.185752575826015</v>
+        <v>1.24184190254812</v>
       </c>
       <c r="F254">
         <v>1</v>
@@ -7019,7 +7019,7 @@
         <v>46.73366779861109</v>
       </c>
       <c r="E255">
-        <v>1.141009926768416</v>
+        <v>1.198136083388974</v>
       </c>
       <c r="F255">
         <v>1</v>
@@ -7045,7 +7045,7 @@
         <v>45.56250372282135</v>
       </c>
       <c r="E256">
-        <v>1.475487968659615</v>
+        <v>1.470728772785298</v>
       </c>
       <c r="F256">
         <v>1</v>
@@ -7071,7 +7071,7 @@
         <v>43.95502361879623</v>
       </c>
       <c r="E257">
-        <v>1.55304603835082</v>
+        <v>1.550939585388147</v>
       </c>
       <c r="F257">
         <v>1</v>
@@ -7097,7 +7097,7 @@
         <v>42.53125552665969</v>
       </c>
       <c r="E258">
-        <v>1.621740328648744</v>
+        <v>1.621983447979243</v>
       </c>
       <c r="F258">
         <v>1</v>
@@ -7123,7 +7123,7 @@
         <v>41.4978754597864</v>
       </c>
       <c r="E259">
-        <v>1.671599087735947</v>
+        <v>1.67354754179536</v>
       </c>
       <c r="F259">
         <v>1</v>
@@ -7149,7 +7149,7 @@
         <v>40.44153139142702</v>
       </c>
       <c r="E260">
-        <v>1.72256581924731</v>
+        <v>1.726257504362948</v>
       </c>
       <c r="F260">
         <v>1</v>
@@ -7175,7 +7175,7 @@
         <v>39.63779133941446</v>
       </c>
       <c r="E261">
-        <v>1.689849361734483</v>
+        <v>1.69601191361769</v>
       </c>
       <c r="F261">
         <v>1</v>
@@ -7201,7 +7201,7 @@
         <v>39.82150335130305</v>
       </c>
       <c r="E262">
-        <v>1.706983943198813</v>
+        <v>1.712427144350184</v>
       </c>
       <c r="F262">
         <v>1</v>
@@ -7227,7 +7227,7 @@
         <v>40.46449539291309</v>
       </c>
       <c r="E263">
-        <v>1.72145784682315</v>
+        <v>1.725111635611478</v>
       </c>
       <c r="F263">
         <v>1</v>
@@ -7253,7 +7253,7 @@
         <v>41.24527144343959</v>
       </c>
       <c r="E264">
-        <v>1.683786784401708</v>
+        <v>1.686152098061523</v>
       </c>
       <c r="F264">
         <v>1</v>
@@ -7279,7 +7279,7 @@
         <v>49.76491599477275</v>
       </c>
       <c r="E265">
-        <v>1.218720843552667</v>
+        <v>1.274046190349597</v>
       </c>
       <c r="F265">
         <v>1</v>
@@ -7305,7 +7305,7 @@
         <v>49.90270000368919</v>
       </c>
       <c r="E266">
-        <v>1.222253157951951</v>
+        <v>1.277496649756898</v>
       </c>
       <c r="F266">
         <v>1</v>
@@ -7331,7 +7331,7 @@
         <v>49.213779959107</v>
       </c>
       <c r="E267">
-        <v>1.20459158595553</v>
+        <v>1.260244352720393</v>
       </c>
       <c r="F267">
         <v>1</v>
@@ -7357,7 +7357,7 @@
         <v>47.97372387885905</v>
       </c>
       <c r="E268">
-        <v>1.172800756361973</v>
+        <v>1.229190218054683</v>
       </c>
       <c r="F268">
         <v>1</v>
@@ -7383,7 +7383,7 @@
         <v>46.77959580158323</v>
       </c>
       <c r="E269">
-        <v>1.142187364901511</v>
+        <v>1.199286236524741</v>
       </c>
       <c r="F269">
         <v>1</v>
@@ -7409,7 +7409,7 @@
         <v>45.44768371539099</v>
       </c>
       <c r="E270">
-        <v>1.481027830780415</v>
+        <v>1.476458116542644</v>
       </c>
       <c r="F270">
         <v>1</v>
@@ -7435,7 +7435,7 @@
         <v>44.39133964703161</v>
       </c>
       <c r="E271">
-        <v>1.531994562291779</v>
+        <v>1.529168079110231</v>
       </c>
       <c r="F271">
         <v>1</v>
@@ -7461,7 +7461,7 @@
         <v>43.10535556381151</v>
       </c>
       <c r="E272">
-        <v>1.594041018044742</v>
+        <v>1.593336729192511</v>
       </c>
       <c r="F272">
         <v>1</v>
@@ -7487,7 +7487,7 @@
         <v>42.18679550436859</v>
       </c>
       <c r="E273">
-        <v>1.638359915011145</v>
+        <v>1.639171479251282</v>
       </c>
       <c r="F273">
         <v>1</v>
@@ -7513,7 +7513,7 @@
         <v>41.17637943898137</v>
       </c>
       <c r="E274">
-        <v>1.687110701674188</v>
+        <v>1.68958970431593</v>
       </c>
       <c r="F274">
         <v>1</v>
@@ -7539,7 +7539,7 @@
         <v>41.52083946127247</v>
       </c>
       <c r="E275">
-        <v>1.670491115311787</v>
+        <v>1.672401673043891</v>
       </c>
       <c r="F275">
         <v>1</v>
@@ -7565,7 +7565,7 @@
         <v>42.20975950585466</v>
       </c>
       <c r="E276">
-        <v>1.637251942586985</v>
+        <v>1.638025610499813</v>
       </c>
       <c r="F276">
         <v>1</v>
@@ -7591,7 +7591,7 @@
         <v>42.69200353706221</v>
       </c>
       <c r="E277">
-        <v>1.613984521679623</v>
+        <v>1.613962366718958</v>
       </c>
       <c r="F277">
         <v>1</v>
@@ -7617,7 +7617,7 @@
         <v>44.02391562325445</v>
       </c>
       <c r="E278">
-        <v>1.54972212107834</v>
+        <v>1.547501979133739</v>
       </c>
       <c r="F278">
         <v>1</v>
@@ -7643,7 +7643,7 @@
         <v>51.30350409433966</v>
       </c>
       <c r="E279">
-        <v>1.258165021011339</v>
+        <v>1.312576320397791</v>
       </c>
       <c r="F279">
         <v>1</v>
@@ -7669,7 +7669,7 @@
         <v>50.86718806610426</v>
       </c>
       <c r="E280">
-        <v>1.24697935874694</v>
+        <v>1.301649865608005</v>
       </c>
       <c r="F280">
         <v>1</v>
@@ -7695,7 +7695,7 @@
         <v>49.8108439977449</v>
       </c>
       <c r="E281">
-        <v>1.219898281685762</v>
+        <v>1.275196343485364</v>
       </c>
       <c r="F281">
         <v>1</v>
@@ -7721,7 +7721,7 @@
         <v>49.05303194870449</v>
       </c>
       <c r="E282">
-        <v>1.200470552489699</v>
+        <v>1.256218816745208</v>
       </c>
       <c r="F282">
         <v>1</v>
@@ -7747,7 +7747,7 @@
         <v>47.4914798476515</v>
       </c>
       <c r="E283">
-        <v>1.160437655964479</v>
+        <v>1.21711361012913</v>
       </c>
       <c r="F283">
         <v>1</v>
@@ -7773,7 +7773,7 @@
         <v>46.36624377483392</v>
       </c>
       <c r="E284">
-        <v>1.195006296686236</v>
+        <v>1.240703248155948</v>
       </c>
       <c r="F284">
         <v>1</v>
@@ -7799,7 +7799,7 @@
         <v>45.30989970647455</v>
       </c>
       <c r="E285">
-        <v>1.487675665325376</v>
+        <v>1.48333332905146</v>
       </c>
       <c r="F285">
         <v>1</v>
@@ -7825,7 +7825,7 @@
         <v>43.74834760542157</v>
       </c>
       <c r="E286">
-        <v>1.56301779016826</v>
+        <v>1.561252404151371</v>
       </c>
       <c r="F286">
         <v>1</v>
@@ -7851,7 +7851,7 @@
         <v>42.73793154003435</v>
       </c>
       <c r="E287">
-        <v>1.611768576831303</v>
+        <v>1.611670629216019</v>
       </c>
       <c r="F287">
         <v>1</v>
@@ -7877,7 +7877,7 @@
         <v>42.69200353706221</v>
       </c>
       <c r="E288">
-        <v>1.613984521679623</v>
+        <v>1.613962366718958</v>
       </c>
       <c r="F288">
         <v>1</v>
@@ -7903,7 +7903,7 @@
         <v>43.35795958015832</v>
       </c>
       <c r="E289">
-        <v>1.581853321378981</v>
+        <v>1.580732172926349</v>
       </c>
       <c r="F289">
         <v>1</v>
@@ -7929,7 +7929,7 @@
         <v>43.93205961731016</v>
       </c>
       <c r="E290">
-        <v>1.55415401077498</v>
+        <v>1.552085454139617</v>
       </c>
       <c r="F290">
         <v>1</v>
@@ -7955,7 +7955,7 @@
         <v>44.71283566783664</v>
       </c>
       <c r="E291">
-        <v>1.516482948353538</v>
+        <v>1.513125916589661</v>
       </c>
       <c r="F291">
         <v>1</v>
@@ -7981,7 +7981,7 @@
         <v>52.52059617310154</v>
       </c>
       <c r="E292">
-        <v>1.289367131538349</v>
+        <v>1.343055378495617</v>
       </c>
       <c r="F292">
         <v>1</v>
@@ -8007,7 +8007,7 @@
         <v>52.33688416121295</v>
       </c>
       <c r="E293">
-        <v>1.28465737900597</v>
+        <v>1.338454765952549</v>
       </c>
       <c r="F293">
         <v>1</v>
@@ -8033,7 +8033,7 @@
         <v>51.16572008542322</v>
       </c>
       <c r="E294">
-        <v>1.254632706612055</v>
+        <v>1.30912586099049</v>
       </c>
       <c r="F294">
         <v>1</v>
@@ -8059,7 +8059,7 @@
         <v>49.30563596505129</v>
       </c>
       <c r="E295">
-        <v>1.20694646222172</v>
+        <v>1.262544658991926</v>
       </c>
       <c r="F295">
         <v>1</v>
@@ -8085,7 +8085,7 @@
         <v>48.29521989966406</v>
       </c>
       <c r="E296">
-        <v>1.181042823293636</v>
+        <v>1.237241290005052</v>
       </c>
       <c r="F296">
         <v>1</v>
@@ -8111,7 +8111,7 @@
         <v>47.05516381941611</v>
       </c>
       <c r="E297">
-        <v>1.149251993700079</v>
+        <v>1.206187155339343</v>
       </c>
       <c r="F297">
         <v>1</v>
@@ -8137,7 +8137,7 @@
         <v>45.5165757198492</v>
       </c>
       <c r="E298">
-        <v>1.477703913507935</v>
+        <v>1.473020510288236</v>
       </c>
       <c r="F298">
         <v>1</v>
@@ -8163,7 +8163,7 @@
         <v>44.16169963217089</v>
       </c>
       <c r="E299">
-        <v>1.543074286533379</v>
+        <v>1.540626766624924</v>
       </c>
       <c r="F299">
         <v>1</v>
@@ -8189,7 +8189,7 @@
         <v>43.77131160690764</v>
       </c>
       <c r="E300">
-        <v>1.5619098177441</v>
+        <v>1.560106535399902</v>
       </c>
       <c r="F300">
         <v>1</v>
@@ -8215,7 +8215,7 @@
         <v>45.0113676871556</v>
       </c>
       <c r="E301">
-        <v>1.502079306839457</v>
+        <v>1.49822962282056</v>
       </c>
       <c r="F301">
         <v>1</v>
@@ -8241,7 +8241,7 @@
         <v>45.56250372282135</v>
       </c>
       <c r="E302">
-        <v>1.475487968659615</v>
+        <v>1.470728772785298</v>
       </c>
       <c r="F302">
         <v>1</v>
@@ -8267,7 +8267,7 @@
         <v>45.70028773173779</v>
       </c>
       <c r="E303">
-        <v>1.468840134114655</v>
+        <v>1.463853560276482</v>
       </c>
       <c r="F303">
         <v>1</v>
@@ -8293,7 +8293,7 @@
         <v>46.50402778375036</v>
       </c>
       <c r="E304">
-        <v>1.135122736102943</v>
+        <v>1.192385317710139</v>
       </c>
       <c r="F304">
         <v>1</v>
@@ -8319,7 +8319,7 @@
         <v>53.89843626226593</v>
       </c>
       <c r="E305">
-        <v>1.32469027553119</v>
+        <v>1.377559972568627</v>
       </c>
       <c r="F305">
         <v>1</v>
@@ -8345,7 +8345,7 @@
         <v>53.6687962474052</v>
       </c>
       <c r="E306">
-        <v>1.318803084865717</v>
+        <v>1.371809206889792</v>
       </c>
       <c r="F306">
         <v>1</v>
@@ -8371,7 +8371,7 @@
         <v>52.88802019687871</v>
       </c>
       <c r="E307">
-        <v>1.298786636603107</v>
+        <v>1.352256603581753</v>
       </c>
       <c r="F307">
         <v>1</v>
@@ -8397,7 +8397,7 @@
         <v>50.22419602449422</v>
       </c>
       <c r="E308">
-        <v>1.230495224883614</v>
+        <v>1.285547721707267</v>
       </c>
       <c r="F308">
         <v>1</v>
@@ -8423,7 +8423,7 @@
         <v>48.38707590560836</v>
       </c>
       <c r="E309">
-        <v>1.183397699559826</v>
+        <v>1.239541596276586</v>
       </c>
       <c r="F309">
         <v>1</v>
@@ -8449,7 +8449,7 @@
         <v>47.46851584616543</v>
       </c>
       <c r="E310">
-        <v>1.159848936897931</v>
+        <v>1.216538533561246</v>
       </c>
       <c r="F310">
         <v>1</v>
@@ -8475,7 +8475,7 @@
         <v>46.15956776145926</v>
       </c>
       <c r="E311">
-        <v>1.303856400055949</v>
+        <v>1.328710660780596</v>
       </c>
       <c r="F311">
         <v>1</v>
@@ -8501,7 +8501,7 @@
         <v>45.05729569012775</v>
       </c>
       <c r="E312">
-        <v>1.499863361991137</v>
+        <v>1.495937885317622</v>
       </c>
       <c r="F312">
         <v>1</v>
@@ -8527,7 +8527,7 @@
         <v>45.47064771687707</v>
       </c>
       <c r="E313">
-        <v>1.479919858356255</v>
+        <v>1.475312247791175</v>
       </c>
       <c r="F313">
         <v>1</v>
@@ -8553,7 +8553,7 @@
         <v>46.54995578672251</v>
       </c>
       <c r="E314">
-        <v>1.136300174236037</v>
+        <v>1.193535470845906</v>
       </c>
       <c r="F314">
         <v>1</v>
@@ -8579,7 +8579,7 @@
         <v>47.9277958758869</v>
       </c>
       <c r="E315">
-        <v>1.171623318228878</v>
+        <v>1.228040064918916</v>
       </c>
       <c r="F315">
         <v>1</v>
@@ -8605,7 +8605,7 @@
         <v>48.11150788777547</v>
       </c>
       <c r="E316">
-        <v>1.176333070761257</v>
+        <v>1.232640677461984</v>
       </c>
       <c r="F316">
         <v>1</v>
@@ -8631,7 +8631,7 @@
         <v>55.09256433954174</v>
       </c>
       <c r="E317">
-        <v>1.355303666991653</v>
+        <v>1.40746395409857</v>
       </c>
       <c r="F317">
         <v>1</v>
@@ -8657,7 +8657,7 @@
         <v>54.17400428009881</v>
       </c>
       <c r="E318">
-        <v>1.331754904329759</v>
+        <v>1.384460891383229</v>
       </c>
       <c r="F318">
         <v>1</v>
@@ -8683,7 +8683,7 @@
         <v>52.97987620282301</v>
       </c>
       <c r="E319">
-        <v>1.301141512869296</v>
+        <v>1.354556909853287</v>
       </c>
       <c r="F319">
         <v>1</v>
@@ -8709,7 +8709,7 @@
         <v>51.32646809582573</v>
       </c>
       <c r="E320">
-        <v>1.258753740077887</v>
+        <v>1.313151396965675</v>
       </c>
       <c r="F320">
         <v>1</v>
@@ -8735,7 +8735,7 @@
         <v>49.76491599477275</v>
       </c>
       <c r="E321">
-        <v>1.218720843552667</v>
+        <v>1.274046190349597</v>
       </c>
       <c r="F321">
         <v>1</v>
@@ -8761,7 +8761,7 @@
         <v>48.13447188926155</v>
       </c>
       <c r="E322">
-        <v>1.176921789827805</v>
+        <v>1.233215754029868</v>
       </c>
       <c r="F322">
         <v>1</v>
@@ -8787,7 +8787,7 @@
         <v>47.2388758313047</v>
       </c>
       <c r="E323">
-        <v>1.153961746232458</v>
+        <v>1.210787767882411</v>
       </c>
       <c r="F323">
         <v>1</v>
@@ -8813,7 +8813,7 @@
         <v>46.27438776888962</v>
       </c>
       <c r="E324">
-        <v>1.243384120406108</v>
+        <v>1.279817653766903</v>
       </c>
       <c r="F324">
         <v>1</v>
@@ -8839,7 +8839,7 @@
         <v>46.73366779861109</v>
       </c>
       <c r="E325">
-        <v>1.141009926768416</v>
+        <v>1.198136083388974</v>
       </c>
       <c r="F325">
         <v>1</v>
@@ -8865,7 +8865,7 @@
         <v>48.66264392344124</v>
       </c>
       <c r="E326">
-        <v>1.190462328358394</v>
+        <v>1.246442515091188</v>
       </c>
       <c r="F326">
         <v>1</v>
@@ -8891,7 +8891,7 @@
         <v>56.42447642573399</v>
       </c>
       <c r="E327">
-        <v>1.389449372851399</v>
+        <v>1.440818395035813</v>
       </c>
       <c r="F327">
         <v>1</v>
@@ -8917,7 +8917,7 @@
         <v>55.59777237223535</v>
       </c>
       <c r="E328">
-        <v>1.368255486455694</v>
+        <v>1.420115638592007</v>
       </c>
       <c r="F328">
         <v>1</v>
@@ -8943,7 +8943,7 @@
         <v>54.5184643023899</v>
       </c>
       <c r="E329">
-        <v>1.340585690327969</v>
+        <v>1.393087039901482</v>
       </c>
       <c r="F329">
         <v>1</v>
@@ -8969,7 +8969,7 @@
         <v>52.58948817755976</v>
       </c>
       <c r="E330">
-        <v>1.291133288737991</v>
+        <v>1.344780608199268</v>
       </c>
       <c r="F330">
         <v>1</v>
@@ -8995,7 +8995,7 @@
         <v>51.16572008542322</v>
       </c>
       <c r="E331">
-        <v>1.254632706612055</v>
+        <v>1.30912586099049</v>
       </c>
       <c r="F331">
         <v>1</v>
@@ -9021,7 +9021,7 @@
         <v>49.44341997396772</v>
       </c>
       <c r="E332">
-        <v>1.210478776621004</v>
+        <v>1.265995118399228</v>
       </c>
       <c r="F332">
         <v>1</v>
@@ -9047,7 +9047,7 @@
         <v>48.96117594276019</v>
       </c>
       <c r="E333">
-        <v>1.198115676223509</v>
+        <v>1.253918510473674</v>
       </c>
       <c r="F333">
         <v>1</v>
@@ -9073,7 +9073,7 @@
         <v>47.99668788034512</v>
       </c>
       <c r="E334">
-        <v>1.173389475428521</v>
+        <v>1.229765294622567</v>
       </c>
       <c r="F334">
         <v>1</v>
@@ -9099,7 +9099,7 @@
         <v>48.06557988480333</v>
       </c>
       <c r="E335">
-        <v>1.175155632628163</v>
+        <v>1.231490524326217</v>
       </c>
       <c r="F335">
         <v>1</v>
@@ -9125,7 +9125,7 @@
         <v>49.83380799923097</v>
       </c>
       <c r="E336">
-        <v>1.220487000752309</v>
+        <v>1.275771420053247</v>
       </c>
       <c r="F336">
         <v>1</v>
@@ -9151,7 +9151,7 @@
         <v>57.68749650746801</v>
       </c>
       <c r="E337">
-        <v>1.421828921511503</v>
+        <v>1.472447606269406</v>
       </c>
       <c r="F337">
         <v>1</v>
@@ -9177,7 +9177,7 @@
         <v>57.66453250598194</v>
       </c>
       <c r="E338">
-        <v>1.421240202444956</v>
+        <v>1.471872529701522</v>
       </c>
       <c r="F338">
         <v>1</v>
@@ -9203,7 +9203,7 @@
         <v>55.2992403529164</v>
       </c>
       <c r="E339">
-        <v>1.360602138590579</v>
+        <v>1.412639643209521</v>
       </c>
       <c r="F339">
         <v>1</v>
@@ -9229,7 +9229,7 @@
         <v>53.59990424294698</v>
       </c>
       <c r="E340">
-        <v>1.317036927666074</v>
+        <v>1.370083977186142</v>
       </c>
       <c r="F340">
         <v>1</v>
@@ -9255,7 +9255,7 @@
         <v>51.99242413892185</v>
       </c>
       <c r="E341">
-        <v>1.27582659300776</v>
+        <v>1.329828617434297</v>
       </c>
       <c r="F341">
         <v>1</v>
@@ -9281,7 +9281,7 @@
         <v>50.93608007056248</v>
       </c>
       <c r="E342">
-        <v>1.248745515946582</v>
+        <v>1.303375095311655</v>
       </c>
       <c r="F342">
         <v>1</v>
@@ -9307,7 +9307,7 @@
         <v>49.99455600963348</v>
       </c>
       <c r="E343">
-        <v>1.22460803421814</v>
+        <v>1.279796956028432</v>
       </c>
       <c r="F343">
         <v>1</v>
@@ -9333,7 +9333,7 @@
         <v>49.25970796207915</v>
       </c>
       <c r="E344">
-        <v>1.205769024088625</v>
+        <v>1.26139450585616</v>
       </c>
       <c r="F344">
         <v>1</v>
@@ -9359,7 +9359,7 @@
         <v>49.30563596505129</v>
       </c>
       <c r="E345">
-        <v>1.20694646222172</v>
+        <v>1.262544658991926</v>
       </c>
       <c r="F345">
         <v>1</v>
@@ -9385,7 +9385,7 @@
         <v>58.69791257285523</v>
       </c>
       <c r="E346">
-        <v>1.447732560439587</v>
+        <v>1.49775097525628</v>
       </c>
       <c r="F346">
         <v>1</v>
@@ -9411,7 +9411,7 @@
         <v>58.12381253570341</v>
       </c>
       <c r="E347">
-        <v>1.433014583775903</v>
+        <v>1.483374061059192</v>
       </c>
       <c r="F347">
         <v>1</v>
@@ -9437,7 +9437,7 @@
         <v>56.53929643316435</v>
       </c>
       <c r="E348">
-        <v>1.392392968184136</v>
+        <v>1.44369377787523</v>
       </c>
       <c r="F348">
         <v>1</v>
@@ -9463,7 +9463,7 @@
         <v>55.11552834102781</v>
       </c>
       <c r="E349">
-        <v>1.3558923860582</v>
+        <v>1.408039030666453</v>
       </c>
       <c r="F349">
         <v>1</v>
@@ -9489,7 +9489,7 @@
         <v>53.04876820728123</v>
       </c>
       <c r="E350">
-        <v>1.302907670068938</v>
+        <v>1.356282139556938</v>
       </c>
       <c r="F350">
         <v>1</v>
@@ -9515,7 +9515,7 @@
         <v>51.90056813297755</v>
       </c>
       <c r="E351">
-        <v>1.273471716741571</v>
+        <v>1.327528311162762</v>
       </c>
       <c r="F351">
         <v>1</v>
@@ -9541,7 +9541,7 @@
         <v>51.05090007799285</v>
       </c>
       <c r="E352">
-        <v>1.251689111279318</v>
+        <v>1.306250478151073</v>
       </c>
       <c r="F352">
         <v>1</v>
@@ -9567,7 +9567,7 @@
         <v>50.56865604678532</v>
       </c>
       <c r="E353">
-        <v>1.239326010881824</v>
+        <v>1.294173870225519</v>
       </c>
       <c r="F353">
         <v>1</v>
@@ -9593,7 +9593,7 @@
         <v>60.0068606575614</v>
       </c>
       <c r="E354">
-        <v>1.481289547232786</v>
+        <v>1.53053033962564</v>
       </c>
       <c r="F354">
         <v>1</v>
@@ -9619,7 +9619,7 @@
         <v>58.65198456988308</v>
       </c>
       <c r="E355">
-        <v>1.446555122306492</v>
+        <v>1.496600822120513</v>
       </c>
       <c r="F355">
         <v>1</v>
@@ -9645,7 +9645,7 @@
         <v>57.25118047923262</v>
       </c>
       <c r="E356">
-        <v>1.410643259247104</v>
+        <v>1.461521151479619</v>
       </c>
       <c r="F356">
         <v>1</v>
@@ -9671,7 +9671,7 @@
         <v>56.12594440641503</v>
       </c>
       <c r="E357">
-        <v>1.381796024986283</v>
+        <v>1.433342399653327</v>
       </c>
       <c r="F357">
         <v>1</v>
@@ -9697,7 +9697,7 @@
         <v>54.0132562696963</v>
       </c>
       <c r="E358">
-        <v>1.327633870863927</v>
+        <v>1.380435355408045</v>
       </c>
       <c r="F358">
         <v>1</v>
@@ -9723,7 +9723,7 @@
         <v>52.56652417607368</v>
       </c>
       <c r="E359">
-        <v>1.290544569671444</v>
+        <v>1.344205531631384</v>
       </c>
       <c r="F359">
         <v>1</v>
@@ -9749,7 +9749,7 @@
         <v>52.26799215675473</v>
       </c>
       <c r="E360">
-        <v>1.282891221806328</v>
+        <v>1.336729536248899</v>
       </c>
       <c r="F360">
         <v>1</v>
@@ -9775,7 +9775,7 @@
         <v>61.01727672294862</v>
       </c>
       <c r="E361">
-        <v>1.507193186160869</v>
+        <v>1.555833708612514</v>
       </c>
       <c r="F361">
         <v>1</v>
@@ -9801,7 +9801,7 @@
         <v>60.19057266944999</v>
       </c>
       <c r="E362">
-        <v>1.485999299765165</v>
+        <v>1.535130952168708</v>
       </c>
       <c r="F362">
         <v>1</v>
@@ -9827,7 +9827,7 @@
         <v>57.73342451044016</v>
       </c>
       <c r="E363">
-        <v>1.423006359644598</v>
+        <v>1.473597759405173</v>
       </c>
       <c r="F363">
         <v>1</v>
@@ -9853,7 +9853,7 @@
         <v>56.79190044951116</v>
       </c>
       <c r="E364">
-        <v>1.398868877916157</v>
+        <v>1.450019620121949</v>
       </c>
       <c r="F364">
         <v>1</v>
@@ -9879,7 +9879,7 @@
         <v>55.16145634399996</v>
       </c>
       <c r="E365">
-        <v>1.357069824191295</v>
+        <v>1.40918918380222</v>
       </c>
       <c r="F365">
         <v>1</v>
@@ -9905,7 +9905,7 @@
         <v>54.44957229793168</v>
       </c>
       <c r="E366">
-        <v>1.338819533128327</v>
+        <v>1.391361810197832</v>
       </c>
       <c r="F366">
         <v>1</v>
@@ -9931,7 +9931,7 @@
         <v>54.56439230536205</v>
       </c>
       <c r="E367">
-        <v>1.341763128461063</v>
+        <v>1.394237193037249</v>
       </c>
       <c r="F367">
         <v>1</v>
@@ -9957,7 +9957,7 @@
         <v>63.29071287006987</v>
       </c>
       <c r="E368">
-        <v>1.565476373749057</v>
+        <v>1.612766288832981</v>
       </c>
       <c r="F368">
         <v>1</v>
@@ -9983,7 +9983,7 @@
         <v>62.14251279576621</v>
       </c>
       <c r="E369">
-        <v>1.53604042042169</v>
+        <v>1.584012460438805</v>
       </c>
       <c r="F369">
         <v>1</v>
@@ -10009,7 +10009,7 @@
         <v>59.52461662635386</v>
       </c>
       <c r="E370">
-        <v>1.468926446835292</v>
+        <v>1.518453731700086</v>
       </c>
       <c r="F370">
         <v>1</v>
@@ -10035,7 +10035,7 @@
         <v>57.73342451044016</v>
       </c>
       <c r="E371">
-        <v>1.423006359644598</v>
+        <v>1.473597759405173</v>
       </c>
       <c r="F371">
         <v>1</v>
@@ -10061,7 +10061,7 @@
         <v>57.06746846734403</v>
       </c>
       <c r="E372">
-        <v>1.405933506714725</v>
+        <v>1.456920538936551</v>
       </c>
       <c r="F372">
         <v>1</v>
@@ -10087,7 +10087,7 @@
         <v>56.86079245396938</v>
       </c>
       <c r="E373">
-        <v>1.400635035115799</v>
+        <v>1.451744849825599</v>
       </c>
       <c r="F373">
         <v>1</v>
@@ -10113,7 +10113,7 @@
         <v>63.33664087304201</v>
       </c>
       <c r="E374">
-        <v>1.566653811882152</v>
+        <v>1.613916441968748</v>
       </c>
       <c r="F374">
         <v>1</v>
@@ -10139,7 +10139,7 @@
         <v>60.92542071700433</v>
       </c>
       <c r="E375">
-        <v>1.50483830989468</v>
+        <v>1.55353340234098</v>
       </c>
       <c r="F375">
         <v>1</v>
@@ -10165,7 +10165,7 @@
         <v>59.43276062040958</v>
       </c>
       <c r="E376">
-        <v>1.466571570569102</v>
+        <v>1.516153425428552</v>
       </c>
       <c r="F376">
         <v>1</v>

</xml_diff>

<commit_message>
bugfix and fertility map
</commit_message>
<xml_diff>
--- a/output_highsierra/xyz_age_eros.xlsx
+++ b/output_highsierra/xyz_age_eros.xlsx
@@ -441,7 +441,7 @@
         <v>20.30210208814082</v>
       </c>
       <c r="E2">
-        <v>3.78300140314787</v>
+        <v>3.676879382165289</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -467,7 +467,7 @@
         <v>21.15177014312552</v>
       </c>
       <c r="E3">
-        <v>3.649849202651979</v>
+        <v>3.561649508784751</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -493,7 +493,7 @@
         <v>20.80731012083443</v>
       </c>
       <c r="E4">
-        <v>3.723822647371918</v>
+        <v>3.625666105107272</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -519,7 +519,7 @@
         <v>20.5776701059737</v>
       </c>
       <c r="E5">
-        <v>3.773138277185212</v>
+        <v>3.668343835988953</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -545,7 +545,7 @@
         <v>22.75925024715065</v>
       </c>
       <c r="E6">
-        <v>3.304639793958926</v>
+        <v>3.262905392612986</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -571,7 +571,7 @@
         <v>22.4607182278317</v>
       </c>
       <c r="E7">
-        <v>3.368750112716207</v>
+        <v>3.318386442759171</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -597,7 +597,7 @@
         <v>21.88661819067987</v>
       </c>
       <c r="E8">
-        <v>3.492039187249441</v>
+        <v>3.425080769963373</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -623,7 +623,7 @@
         <v>24.435622355634</v>
       </c>
       <c r="E9">
-        <v>2.944635696321886</v>
+        <v>2.951357957176717</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -649,7 +649,7 @@
         <v>23.86152231848217</v>
       </c>
       <c r="E10">
-        <v>3.067924770855119</v>
+        <v>3.058052284380919</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -675,7 +675,7 @@
         <v>23.54002629767714</v>
       </c>
       <c r="E11">
-        <v>3.136966652593729</v>
+        <v>3.117801107615272</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -701,7 +701,7 @@
         <v>22.4607182278317</v>
       </c>
       <c r="E12">
-        <v>3.368750112716207</v>
+        <v>3.318386442759171</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -727,7 +727,7 @@
         <v>25.79049844331232</v>
       </c>
       <c r="E13">
-        <v>2.653673480423457</v>
+        <v>2.699559344974801</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -753,7 +753,7 @@
         <v>26.41052648343629</v>
       </c>
       <c r="E14">
-        <v>2.520521279927565</v>
+        <v>2.584329471594263</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -779,7 +779,7 @@
         <v>26.20385047006163</v>
       </c>
       <c r="E15">
-        <v>2.564905346759529</v>
+        <v>2.622739429387775</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -805,7 +805,7 @@
         <v>24.7800823779251</v>
       </c>
       <c r="E16">
-        <v>2.870662251601947</v>
+        <v>2.887341360854196</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -831,7 +831,7 @@
         <v>23.70077430807965</v>
       </c>
       <c r="E17">
-        <v>3.102445711724425</v>
+        <v>3.087926695998095</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -857,7 +857,7 @@
         <v>22.27700621594312</v>
       </c>
       <c r="E18">
-        <v>3.408202616566842</v>
+        <v>3.352528627464516</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -883,7 +883,7 @@
         <v>27.03055452356027</v>
       </c>
       <c r="E19">
-        <v>2.387369079431673</v>
+        <v>2.469099598213725</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -909,7 +909,7 @@
         <v>27.12241052950456</v>
       </c>
       <c r="E20">
-        <v>2.367642827506356</v>
+        <v>2.452028505861053</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -935,7 +935,7 @@
         <v>27.12241052950456</v>
       </c>
       <c r="E21">
-        <v>2.367642827506356</v>
+        <v>2.452028505861053</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -961,7 +961,7 @@
         <v>26.41052648343629</v>
       </c>
       <c r="E22">
-        <v>2.520521279927565</v>
+        <v>2.584329471594263</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -987,7 +987,7 @@
         <v>24.71119037346688</v>
       </c>
       <c r="E23">
-        <v>2.885456940545934</v>
+        <v>2.9001446801187</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>23.7467023110518</v>
       </c>
       <c r="E24">
-        <v>3.092582585761766</v>
+        <v>3.079391149821759</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1039,7 +1039,7 @@
         <v>22.43775422634562</v>
       </c>
       <c r="E25">
-        <v>3.373681675697537</v>
+        <v>3.322654215847339</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1065,7 +1065,7 @@
         <v>28.04097058894749</v>
       </c>
       <c r="E26">
-        <v>2.170380308253184</v>
+        <v>2.28131758233433</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1091,7 +1091,7 @@
         <v>28.01800658746141</v>
       </c>
       <c r="E27">
-        <v>2.175311871234513</v>
+        <v>2.285585355422498</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1117,7 +1117,7 @@
         <v>27.85725857705891</v>
       </c>
       <c r="E28">
-        <v>2.209832812103818</v>
+        <v>2.315459767039674</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1143,7 +1143,7 @@
         <v>27.30612254139315</v>
       </c>
       <c r="E29">
-        <v>2.328190323655722</v>
+        <v>2.417886321155708</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1169,7 +1169,7 @@
         <v>25.88235444925661</v>
       </c>
       <c r="E30">
-        <v>2.633947228498139</v>
+        <v>2.682488252622129</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -1195,7 +1195,7 @@
         <v>24.55044236306436</v>
       </c>
       <c r="E31">
-        <v>2.91997788141524</v>
+        <v>2.930019091735876</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -1221,7 +1221,7 @@
         <v>23.79263031402395</v>
       </c>
       <c r="E32">
-        <v>3.082719459799107</v>
+        <v>3.070855603645423</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -1247,7 +1247,7 @@
         <v>23.21853027687212</v>
       </c>
       <c r="E33">
-        <v>3.20600853433234</v>
+        <v>3.177549930849625</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -1273,7 +1273,7 @@
         <v>29.55659468702832</v>
       </c>
       <c r="E34">
-        <v>2.201243596058931</v>
+        <v>2.146394104353154</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1299,7 +1299,7 @@
         <v>29.21213466473723</v>
       </c>
       <c r="E35">
-        <v>2.236995833493242</v>
+        <v>2.181718195263597</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1325,7 +1325,7 @@
         <v>28.59210662461325</v>
       </c>
       <c r="E36">
-        <v>2.301349860875002</v>
+        <v>2.245301558902396</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1351,7 +1351,7 @@
         <v>27.76540257111461</v>
       </c>
       <c r="E37">
-        <v>2.229559064029135</v>
+        <v>2.332530859392347</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -1377,7 +1377,7 @@
         <v>26.0660664611452</v>
       </c>
       <c r="E38">
-        <v>2.594494724647505</v>
+        <v>2.648346067916784</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1403,7 +1403,7 @@
         <v>24.87193838386938</v>
       </c>
       <c r="E39">
-        <v>2.850935999676629</v>
+        <v>2.870270268501524</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1429,7 +1429,7 @@
         <v>23.72373830956573</v>
       </c>
       <c r="E40">
-        <v>3.097514148743095</v>
+        <v>3.083658922909927</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1455,7 +1455,7 @@
         <v>23.93041432294039</v>
       </c>
       <c r="E41">
-        <v>3.053130081911131</v>
+        <v>3.045248965116415</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -1481,7 +1481,7 @@
         <v>24.52747836157829</v>
       </c>
       <c r="E42">
-        <v>2.924909444396569</v>
+        <v>2.934286864824045</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -1507,7 +1507,7 @@
         <v>31.34778680294203</v>
       </c>
       <c r="E43">
-        <v>2.015331961400515</v>
+        <v>1.962708831618847</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -1533,7 +1533,7 @@
         <v>30.7736867657902</v>
       </c>
       <c r="E44">
-        <v>2.074919023791033</v>
+        <v>2.021582316469586</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -1559,7 +1559,7 @@
         <v>29.87809070783335</v>
       </c>
       <c r="E45">
-        <v>2.167874841120241</v>
+        <v>2.113424952836739</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -1585,7 +1585,7 @@
         <v>28.22468260083608</v>
       </c>
       <c r="E46">
-        <v>2.339485580804933</v>
+        <v>2.282980589206869</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -1611,7 +1611,7 @@
         <v>27.19130253396278</v>
       </c>
       <c r="E47">
-        <v>2.352848138562368</v>
+        <v>2.439225186596548</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -1637,7 +1637,7 @@
         <v>25.51493042547943</v>
       </c>
       <c r="E48">
-        <v>2.712852236199408</v>
+        <v>2.750772622032818</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -1663,7 +1663,7 @@
         <v>24.38969435266185</v>
       </c>
       <c r="E49">
-        <v>2.954498822284545</v>
+        <v>2.959893503353053</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -1689,7 +1689,7 @@
         <v>24.52747836157829</v>
       </c>
       <c r="E50">
-        <v>2.924909444396569</v>
+        <v>2.934286864824045</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -1715,7 +1715,7 @@
         <v>24.9408303883276</v>
       </c>
       <c r="E51">
-        <v>2.836141310732641</v>
+        <v>2.857466949237019</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -1741,7 +1741,7 @@
         <v>25.83642644628446</v>
       </c>
       <c r="E52">
-        <v>2.643810354460798</v>
+        <v>2.691023798798465</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -1767,7 +1767,7 @@
         <v>33.48343894114684</v>
       </c>
       <c r="E53">
-        <v>1.793668089307787</v>
+        <v>1.743699467974096</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -1793,7 +1793,7 @@
         <v>32.70266289062035</v>
       </c>
       <c r="E54">
-        <v>1.874706494158892</v>
+        <v>1.823767407371102</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -1819,7 +1819,7 @@
         <v>31.78410283117743</v>
       </c>
       <c r="E55">
-        <v>1.970045793983721</v>
+        <v>1.917964983132285</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -1845,7 +1845,7 @@
         <v>31.48557081185847</v>
       </c>
       <c r="E56">
-        <v>2.00103106642679</v>
+        <v>1.948579195254669</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -1871,7 +1871,7 @@
         <v>30.06180271972193</v>
       </c>
       <c r="E57">
-        <v>2.148806981155275</v>
+        <v>2.094585437684503</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -1897,7 +1897,7 @@
         <v>28.6380346275854</v>
       </c>
       <c r="E58">
-        <v>2.29658289588376</v>
+        <v>2.240591680114337</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -1923,7 +1923,7 @@
         <v>27.23723053693493</v>
       </c>
       <c r="E59">
-        <v>2.342985012599709</v>
+        <v>2.430689640420212</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -1949,7 +1949,7 @@
         <v>25.58382242993765</v>
       </c>
       <c r="E60">
-        <v>2.69805754725542</v>
+        <v>2.737969302768313</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -1975,7 +1975,7 @@
         <v>25.05565039575797</v>
       </c>
       <c r="E61">
-        <v>2.811483495825994</v>
+        <v>2.836128083796179</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2001,7 +2001,7 @@
         <v>25.44603842102122</v>
       </c>
       <c r="E62">
-        <v>2.727646925143397</v>
+        <v>2.763575941297322</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2027,7 +2027,7 @@
         <v>25.85939044777054</v>
       </c>
       <c r="E63">
-        <v>2.638878791479469</v>
+        <v>2.686756025710296</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2053,7 +2053,7 @@
         <v>35.66501908232379</v>
       </c>
       <c r="E64">
-        <v>1.567237252223818</v>
+        <v>1.519980225541286</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2079,7 +2079,7 @@
         <v>34.65460301693658</v>
       </c>
       <c r="E65">
-        <v>1.67211048203113</v>
+        <v>1.623597558878588</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2105,7 +2105,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E66">
-        <v>1.841337739220201</v>
+        <v>1.790798255854688</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2131,7 +2131,7 @@
         <v>32.24338286089889</v>
       </c>
       <c r="E67">
-        <v>1.922376144071306</v>
+        <v>1.870866195251693</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2157,7 +2157,7 @@
         <v>31.18703879253952</v>
       </c>
       <c r="E68">
-        <v>2.03201633886986</v>
+        <v>1.979193407377054</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2183,7 +2183,7 @@
         <v>30.15365872566623</v>
       </c>
       <c r="E69">
-        <v>2.139273051172792</v>
+        <v>2.085165680108385</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2209,7 +2209,7 @@
         <v>28.20171859935</v>
       </c>
       <c r="E70">
-        <v>2.302705588505786</v>
+        <v>2.280087323979461</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2235,7 +2235,7 @@
         <v>26.89277051464383</v>
       </c>
       <c r="E71">
-        <v>2.416958457319649</v>
+        <v>2.494706236742733</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2261,7 +2261,7 @@
         <v>25.6297504329098</v>
       </c>
       <c r="E72">
-        <v>2.688194421292762</v>
+        <v>2.729433756591977</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2287,7 +2287,7 @@
         <v>25.65271443439588</v>
       </c>
       <c r="E73">
-        <v>2.683262858311433</v>
+        <v>2.725165983503809</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -2313,7 +2313,7 @@
         <v>26.64016649829703</v>
       </c>
       <c r="E74">
-        <v>2.471205650114272</v>
+        <v>2.541651740712582</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -2339,7 +2339,7 @@
         <v>27.53576255625388</v>
       </c>
       <c r="E75">
-        <v>2.278874693842428</v>
+        <v>2.375208590274028</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -2365,7 +2365,7 @@
         <v>35.84873109421238</v>
       </c>
       <c r="E76">
-        <v>1.548169392258852</v>
+        <v>1.501140710389049</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -2391,7 +2391,7 @@
         <v>36.53765113879458</v>
       </c>
       <c r="E77">
-        <v>1.47666491739023</v>
+        <v>1.430492528568162</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -2417,7 +2417,7 @@
         <v>35.04499104219982</v>
       </c>
       <c r="E78">
-        <v>1.631591279605578</v>
+        <v>1.583563589180085</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -2443,7 +2443,7 @@
         <v>33.29972692925826</v>
       </c>
       <c r="E79">
-        <v>1.812735949272753</v>
+        <v>1.762538983126333</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -2469,7 +2469,7 @@
         <v>32.08263485049638</v>
       </c>
       <c r="E80">
-        <v>1.939060521540651</v>
+        <v>1.8873507710099</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -2495,7 +2495,7 @@
         <v>31.09518278659523</v>
       </c>
       <c r="E81">
-        <v>2.041550268852343</v>
+        <v>1.988613164953172</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -2521,7 +2521,7 @@
         <v>29.30399067068151</v>
       </c>
       <c r="E82">
-        <v>2.227461903510759</v>
+        <v>2.172298437687479</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -2547,7 +2547,7 @@
         <v>28.2935746052943</v>
       </c>
       <c r="E83">
-        <v>2.332335133318071</v>
+        <v>2.27591577102478</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -2573,7 +2573,7 @@
         <v>26.47941848789451</v>
       </c>
       <c r="E84">
-        <v>2.505726590983577</v>
+        <v>2.571526152329759</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -2599,7 +2599,7 @@
         <v>26.08903046263127</v>
       </c>
       <c r="E85">
-        <v>2.589563161666176</v>
+        <v>2.644078294828616</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -2625,7 +2625,7 @@
         <v>26.86980651315776</v>
       </c>
       <c r="E86">
-        <v>2.421890020300979</v>
+        <v>2.498974009830901</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -2651,7 +2651,7 @@
         <v>28.04097058894749</v>
       </c>
       <c r="E87">
-        <v>2.170380308253184</v>
+        <v>2.28131758233433</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -2677,7 +2677,7 @@
         <v>28.86767464244613</v>
       </c>
       <c r="E88">
-        <v>2.272748070927553</v>
+        <v>2.217042286174041</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -2703,7 +2703,7 @@
         <v>37.08878717446034</v>
       </c>
       <c r="E89">
-        <v>1.46825058720434</v>
+        <v>1.422394792631277</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -2729,7 +2729,7 @@
         <v>37.24953518486285</v>
       </c>
       <c r="E90">
-        <v>1.482613914095272</v>
+        <v>1.436723459294776</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -2755,7 +2755,7 @@
         <v>34.65460301693658</v>
       </c>
       <c r="E91">
-        <v>1.67211048203113</v>
+        <v>1.623597558878588</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -2781,7 +2781,7 @@
         <v>33.6901149545215</v>
       </c>
       <c r="E92">
-        <v>1.7722167468472</v>
+        <v>1.72250501342783</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -2807,7 +2807,7 @@
         <v>31.87595883712171</v>
       </c>
       <c r="E93">
-        <v>1.960511864001238</v>
+        <v>1.908545225556166</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -2833,7 +2833,7 @@
         <v>30.84257877024842</v>
       </c>
       <c r="E94">
-        <v>2.067768576304171</v>
+        <v>2.014517498287498</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -2859,7 +2859,7 @@
         <v>29.21213466473723</v>
       </c>
       <c r="E95">
-        <v>2.236995833493242</v>
+        <v>2.181718195263597</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -2885,7 +2885,7 @@
         <v>27.90318658003105</v>
       </c>
       <c r="E96">
-        <v>2.199969686141159</v>
+        <v>2.306924220863338</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -2911,7 +2911,7 @@
         <v>27.07648252653242</v>
       </c>
       <c r="E97">
-        <v>2.377505953469015</v>
+        <v>2.460564052037389</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -2937,7 +2937,7 @@
         <v>27.51279855476781</v>
       </c>
       <c r="E98">
-        <v>2.283806256823758</v>
+        <v>2.379476363362195</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -2963,7 +2963,7 @@
         <v>28.31653860678037</v>
       </c>
       <c r="E99">
-        <v>2.32995165082245</v>
+        <v>2.273560831630751</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -2989,7 +2989,7 @@
         <v>29.4877026825701</v>
       </c>
       <c r="E100">
-        <v>2.208394043545793</v>
+        <v>2.153458922535243</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3015,7 +3015,7 @@
         <v>30.56701075241554</v>
       </c>
       <c r="E101">
-        <v>2.096370366251619</v>
+        <v>2.042776771015852</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -3041,7 +3041,7 @@
         <v>38.00734723390327</v>
       </c>
       <c r="E102">
-        <v>1.550326740866808</v>
+        <v>1.504272887851273</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -3067,7 +3067,7 @@
         <v>38.4895912651108</v>
       </c>
       <c r="E103">
-        <v>1.593416721539604</v>
+        <v>1.547258887841771</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -3093,7 +3093,7 @@
         <v>37.18064318040463</v>
       </c>
       <c r="E104">
-        <v>1.476458202570587</v>
+        <v>1.430582602153276</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3119,7 +3119,7 @@
         <v>33.91975496938223</v>
       </c>
       <c r="E105">
-        <v>1.748381921890993</v>
+        <v>1.698955619487534</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3145,7 +3145,7 @@
         <v>32.93230290548109</v>
       </c>
       <c r="E106">
-        <v>1.850871669202684</v>
+        <v>1.800218013430806</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3171,7 +3171,7 @@
         <v>31.14111078956738</v>
       </c>
       <c r="E107">
-        <v>2.036783303861101</v>
+        <v>1.983903286165113</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3197,7 +3197,7 @@
         <v>29.80919870337513</v>
       </c>
       <c r="E108">
-        <v>2.175025288607103</v>
+        <v>2.120489771018828</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -3223,7 +3223,7 @@
         <v>28.45432261569681</v>
       </c>
       <c r="E109">
-        <v>2.315650755848726</v>
+        <v>2.259431195266573</v>
       </c>
       <c r="F109">
         <v>1</v>
@@ -3249,7 +3249,7 @@
         <v>27.71947456814247</v>
       </c>
       <c r="E110">
-        <v>2.239422189991794</v>
+        <v>2.341066405568683</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -3275,7 +3275,7 @@
         <v>27.92615058151713</v>
       </c>
       <c r="E111">
-        <v>2.19503812315983</v>
+        <v>2.30265644777517</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -3301,7 +3301,7 @@
         <v>29.21213466473723</v>
       </c>
       <c r="E112">
-        <v>2.236995833493242</v>
+        <v>2.181718195263597</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -3327,7 +3327,7 @@
         <v>30.33737073755481</v>
       </c>
       <c r="E113">
-        <v>2.120205191207826</v>
+        <v>2.066326164956148</v>
       </c>
       <c r="F113">
         <v>1</v>
@@ -3353,7 +3353,7 @@
         <v>31.1181467880813</v>
       </c>
       <c r="E114">
-        <v>2.039166786356722</v>
+        <v>1.986258225559143</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -3379,7 +3379,7 @@
         <v>39.38518732306765</v>
       </c>
       <c r="E115">
-        <v>1.673440971360511</v>
+        <v>1.627090030681267</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -3405,7 +3405,7 @@
         <v>39.06369130226264</v>
       </c>
       <c r="E116">
-        <v>1.644714317578647</v>
+        <v>1.598432697354268</v>
       </c>
       <c r="F116">
         <v>1</v>
@@ -3431,7 +3431,7 @@
         <v>36.67543514771102</v>
       </c>
       <c r="E117">
-        <v>1.462364022416506</v>
+        <v>1.416362892203985</v>
       </c>
       <c r="F117">
         <v>1</v>
@@ -3457,7 +3457,7 @@
         <v>33.64418695154936</v>
       </c>
       <c r="E118">
-        <v>1.776983711838442</v>
+        <v>1.727214892215889</v>
       </c>
       <c r="F118">
         <v>1</v>
@@ -3483,7 +3483,7 @@
         <v>32.67969888913428</v>
       </c>
       <c r="E119">
-        <v>1.877089976654512</v>
+        <v>1.826122346765131</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -3509,7 +3509,7 @@
         <v>31.32482280145596</v>
       </c>
       <c r="E120">
-        <v>2.017715443896135</v>
+        <v>1.965063771012876</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -3535,7 +3535,7 @@
         <v>29.85512670634728</v>
       </c>
       <c r="E121">
-        <v>2.170258323615862</v>
+        <v>2.115779892230769</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -3561,7 +3561,7 @@
         <v>28.86767464244613</v>
       </c>
       <c r="E122">
-        <v>2.272748070927553</v>
+        <v>2.217042286174041</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -3587,7 +3587,7 @@
         <v>29.07435065582079</v>
       </c>
       <c r="E123">
-        <v>2.251296728466966</v>
+        <v>2.195847831627775</v>
       </c>
       <c r="F123">
         <v>1</v>
@@ -3613,7 +3613,7 @@
         <v>29.60252269000047</v>
       </c>
       <c r="E124">
-        <v>2.19647663106769</v>
+        <v>2.141684225565095</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -3639,7 +3639,7 @@
         <v>30.7736867657902</v>
       </c>
       <c r="E125">
-        <v>2.074919023791033</v>
+        <v>2.021582316469586</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -3665,7 +3665,7 @@
         <v>31.83003083414957</v>
       </c>
       <c r="E126">
-        <v>1.965278828992479</v>
+        <v>1.913255104344226</v>
       </c>
       <c r="F126">
         <v>1</v>
@@ -3691,7 +3691,7 @@
         <v>39.95928736021949</v>
       </c>
       <c r="E127">
-        <v>1.724738567399554</v>
+        <v>1.678263840193764</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -3717,7 +3717,7 @@
         <v>40.51042339588524</v>
       </c>
       <c r="E128">
-        <v>1.72281989810854</v>
+        <v>1.679050893055951</v>
       </c>
       <c r="F128">
         <v>1</v>
@@ -3743,7 +3743,7 @@
         <v>39.04072730077657</v>
       </c>
       <c r="E129">
-        <v>1.642662413737086</v>
+        <v>1.596385744973768</v>
       </c>
       <c r="F129">
         <v>1</v>
@@ -3769,7 +3769,7 @@
         <v>35.77983908975416</v>
       </c>
       <c r="E130">
-        <v>1.555319839745714</v>
+        <v>1.508205528571138</v>
       </c>
       <c r="F130">
         <v>1</v>
@@ -3795,7 +3795,7 @@
         <v>33.80493496195187</v>
       </c>
       <c r="E131">
-        <v>1.760299334369097</v>
+        <v>1.710730316457682</v>
       </c>
       <c r="F131">
         <v>1</v>
@@ -3821,7 +3821,7 @@
         <v>32.63377088616213</v>
       </c>
       <c r="E132">
-        <v>1.881856941645754</v>
+        <v>1.83083222555319</v>
       </c>
       <c r="F132">
         <v>1</v>
@@ -3847,7 +3847,7 @@
         <v>30.72775876281806</v>
       </c>
       <c r="E133">
-        <v>2.079685988782274</v>
+        <v>2.026292195257645</v>
       </c>
       <c r="F133">
         <v>1</v>
@@ -3873,7 +3873,7 @@
         <v>29.90105470931942</v>
       </c>
       <c r="E134">
-        <v>2.16549135862462</v>
+        <v>2.11107001344271</v>
       </c>
       <c r="F134">
         <v>1</v>
@@ -3899,7 +3899,7 @@
         <v>30.03883871823586</v>
       </c>
       <c r="E135">
-        <v>2.151190463650896</v>
+        <v>2.096940377078533</v>
       </c>
       <c r="F135">
         <v>1</v>
@@ -3925,7 +3925,7 @@
         <v>30.24551473161052</v>
       </c>
       <c r="E136">
-        <v>2.129739121190309</v>
+        <v>2.075745922532267</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -3951,7 +3951,7 @@
         <v>30.54404675092947</v>
       </c>
       <c r="E137">
-        <v>2.09875384874724</v>
+        <v>2.045131710409882</v>
       </c>
       <c r="F137">
         <v>1</v>
@@ -3977,7 +3977,7 @@
         <v>31.55446281631669</v>
       </c>
       <c r="E138">
-        <v>1.993880618939928</v>
+        <v>1.94151437707258</v>
       </c>
       <c r="F138">
         <v>1</v>
@@ -4003,7 +4003,7 @@
         <v>32.81748289805072</v>
       </c>
       <c r="E139">
-        <v>1.862789081680788</v>
+        <v>1.811992710400954</v>
       </c>
       <c r="F139">
         <v>1</v>
@@ -4029,7 +4029,7 @@
         <v>41.77344347761927</v>
       </c>
       <c r="E140">
-        <v>1.659797116777729</v>
+        <v>1.625465196805969</v>
       </c>
       <c r="F140">
         <v>1</v>
@@ -4055,7 +4055,7 @@
         <v>42.20975950585466</v>
       </c>
       <c r="E141">
-        <v>1.638025610499813</v>
+        <v>1.606953774465066</v>
       </c>
       <c r="F141">
         <v>1</v>
@@ -4081,7 +4081,7 @@
         <v>39.7755753483309</v>
       </c>
       <c r="E142">
-        <v>1.708323336667061</v>
+        <v>1.661888221149765</v>
       </c>
       <c r="F142">
         <v>1</v>
@@ -4107,7 +4107,7 @@
         <v>37.96141923093112</v>
       </c>
       <c r="E143">
-        <v>1.546222933183685</v>
+        <v>1.500178983090273</v>
       </c>
       <c r="F143">
         <v>1</v>
@@ -4133,7 +4133,7 @@
         <v>35.45834306894914</v>
       </c>
       <c r="E144">
-        <v>1.588688594684404</v>
+        <v>1.541174680087552</v>
       </c>
       <c r="F144">
         <v>1</v>
@@ -4159,7 +4159,7 @@
         <v>33.50640294263292</v>
       </c>
       <c r="E145">
-        <v>1.791284606812166</v>
+        <v>1.741344528580066</v>
       </c>
       <c r="F145">
         <v>1</v>
@@ -4185,7 +4185,7 @@
         <v>32.35820286832926</v>
       </c>
       <c r="E146">
-        <v>1.910458731593202</v>
+        <v>1.859091498281545</v>
       </c>
       <c r="F146">
         <v>1</v>
@@ -4211,7 +4211,7 @@
         <v>30.8655427717345</v>
       </c>
       <c r="E147">
-        <v>2.06538509380855</v>
+        <v>2.012162558893468</v>
       </c>
       <c r="F147">
         <v>1</v>
@@ -4237,7 +4237,7 @@
         <v>30.7736867657902</v>
       </c>
       <c r="E148">
-        <v>2.074919023791033</v>
+        <v>2.021582316469586</v>
       </c>
       <c r="F148">
         <v>1</v>
@@ -4263,7 +4263,7 @@
         <v>31.27889479848381</v>
       </c>
       <c r="E149">
-        <v>2.022482408887377</v>
+        <v>1.969773649800935</v>
       </c>
       <c r="F149">
         <v>1</v>
@@ -4289,7 +4289,7 @@
         <v>31.62335482077491</v>
       </c>
       <c r="E150">
-        <v>1.986730171453066</v>
+        <v>1.934449558890492</v>
       </c>
       <c r="F150">
         <v>1</v>
@@ -4315,7 +4315,7 @@
         <v>32.17449085644067</v>
       </c>
       <c r="E151">
-        <v>1.929526591558168</v>
+        <v>1.877931013433782</v>
       </c>
       <c r="F151">
         <v>1</v>
@@ -4341,7 +4341,7 @@
         <v>33.07008691439753</v>
       </c>
       <c r="E152">
-        <v>1.83657077422896</v>
+        <v>1.786088377066628</v>
       </c>
       <c r="F152">
         <v>1</v>
@@ -4367,7 +4367,7 @@
         <v>33.87382696641009</v>
       </c>
       <c r="E153">
-        <v>1.753148886882235</v>
+        <v>1.703665498275593</v>
       </c>
       <c r="F153">
         <v>1</v>
@@ -4393,7 +4393,7 @@
         <v>43.31203157718618</v>
       </c>
       <c r="E154">
-        <v>1.583023910429287</v>
+        <v>1.560188075919627</v>
       </c>
       <c r="F154">
         <v>1</v>
@@ -4419,7 +4419,7 @@
         <v>42.18679550436859</v>
       </c>
       <c r="E155">
-        <v>1.639171479251282</v>
+        <v>1.607928059851429</v>
       </c>
       <c r="F155">
         <v>1</v>
@@ -4445,7 +4445,7 @@
         <v>39.08665530374871</v>
       </c>
       <c r="E156">
-        <v>1.646766221420209</v>
+        <v>1.600479649734768</v>
       </c>
       <c r="F156">
         <v>1</v>
@@ -4471,7 +4471,7 @@
         <v>37.36435519229322</v>
       </c>
       <c r="E157">
-        <v>1.49287343330308</v>
+        <v>1.446958221197275</v>
       </c>
       <c r="F157">
         <v>1</v>
@@ -4497,7 +4497,7 @@
         <v>34.86127903031124</v>
       </c>
       <c r="E158">
-        <v>1.650659139570543</v>
+        <v>1.602403104332321</v>
       </c>
       <c r="F158">
         <v>1</v>
@@ -4523,7 +4523,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E159">
-        <v>1.841337739220201</v>
+        <v>1.790798255854688</v>
       </c>
       <c r="F159">
         <v>1</v>
@@ -4549,7 +4549,7 @@
         <v>32.26634686238496</v>
       </c>
       <c r="E160">
-        <v>1.919992661575685</v>
+        <v>1.868511255857664</v>
       </c>
       <c r="F160">
         <v>1</v>
@@ -4575,7 +4575,7 @@
         <v>31.50853481334455</v>
       </c>
       <c r="E161">
-        <v>1.998647583931169</v>
+        <v>1.94622425586064</v>
       </c>
       <c r="F161">
         <v>1</v>
@@ -4601,7 +4601,7 @@
         <v>31.85299483563564</v>
       </c>
       <c r="E162">
-        <v>1.962895346496859</v>
+        <v>1.910900164950196</v>
       </c>
       <c r="F162">
         <v>1</v>
@@ -4627,7 +4627,7 @@
         <v>32.49598687724569</v>
       </c>
       <c r="E163">
-        <v>1.896157836619478</v>
+        <v>1.844961861917368</v>
       </c>
       <c r="F163">
         <v>1</v>
@@ -4653,7 +4653,7 @@
         <v>33.07008691439753</v>
       </c>
       <c r="E164">
-        <v>1.83657077422896</v>
+        <v>1.786088377066628</v>
       </c>
       <c r="F164">
         <v>1</v>
@@ -4679,7 +4679,7 @@
         <v>33.85086296492401</v>
       </c>
       <c r="E165">
-        <v>1.755532369377855</v>
+        <v>1.706020437669623</v>
       </c>
       <c r="F165">
         <v>1</v>
@@ -4705,7 +4705,7 @@
         <v>34.33310699613155</v>
       </c>
       <c r="E166">
-        <v>1.70547923696982</v>
+        <v>1.656566710395002</v>
       </c>
       <c r="F166">
         <v>1</v>
@@ -4731,7 +4731,7 @@
         <v>43.2890675757001</v>
       </c>
       <c r="E167">
-        <v>1.584169779180757</v>
+        <v>1.56116236130599</v>
       </c>
       <c r="F167">
         <v>1</v>
@@ -4757,7 +4757,7 @@
         <v>43.90909561582409</v>
       </c>
       <c r="E168">
-        <v>1.553231322891086</v>
+        <v>1.534856655874181</v>
       </c>
       <c r="F168">
         <v>1</v>
@@ -4783,7 +4783,7 @@
         <v>42.82978754597865</v>
       </c>
       <c r="E169">
-        <v>1.607087154210142</v>
+        <v>1.580648069033256</v>
       </c>
       <c r="F169">
         <v>1</v>
@@ -4809,7 +4809,7 @@
         <v>38.09920323984756</v>
       </c>
       <c r="E170">
-        <v>1.558534356233055</v>
+        <v>1.512460697373272</v>
       </c>
       <c r="F170">
         <v>1</v>
@@ -4835,7 +4835,7 @@
         <v>36.90507516257176</v>
       </c>
       <c r="E171">
-        <v>1.451835356471846</v>
+        <v>1.406019173587277</v>
       </c>
       <c r="F171">
         <v>1</v>
@@ -4861,7 +4861,7 @@
         <v>34.28717899315941</v>
       </c>
       <c r="E172">
-        <v>1.710246201961061</v>
+        <v>1.661276589183061</v>
       </c>
       <c r="F172">
         <v>1</v>
@@ -4887,7 +4887,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E173">
-        <v>1.841337739220201</v>
+        <v>1.790798255854688</v>
       </c>
       <c r="F173">
         <v>1</v>
@@ -4913,7 +4913,7 @@
         <v>32.88637490250894</v>
       </c>
       <c r="E174">
-        <v>1.855638634193926</v>
+        <v>1.804927892218865</v>
       </c>
       <c r="F174">
         <v>1</v>
@@ -4939,7 +4939,7 @@
         <v>33.02415891142538</v>
       </c>
       <c r="E175">
-        <v>1.841337739220201</v>
+        <v>1.790798255854688</v>
       </c>
       <c r="F175">
         <v>1</v>
@@ -4965,7 +4965,7 @@
         <v>33.48343894114684</v>
       </c>
       <c r="E176">
-        <v>1.793668089307787</v>
+        <v>1.743699467974096</v>
       </c>
       <c r="F176">
         <v>1</v>
@@ -4991,7 +4991,7 @@
         <v>34.0345749768126</v>
       </c>
       <c r="E177">
-        <v>1.736464509412889</v>
+        <v>1.687180922517386</v>
       </c>
       <c r="F177">
         <v>1</v>
@@ -5017,7 +5017,7 @@
         <v>34.6316390154505</v>
       </c>
       <c r="E178">
-        <v>1.67449396452675</v>
+        <v>1.625952498272617</v>
       </c>
       <c r="F178">
         <v>1</v>
@@ -5043,7 +5043,7 @@
         <v>44.46023165148983</v>
       </c>
       <c r="E179">
-        <v>1.525730472855823</v>
+        <v>1.511473806601461</v>
       </c>
       <c r="F179">
         <v>1</v>
@@ -5069,7 +5069,7 @@
         <v>45.14915169607204</v>
       </c>
       <c r="E180">
-        <v>1.491354410311745</v>
+        <v>1.482245245010562</v>
       </c>
       <c r="F180">
         <v>1</v>
@@ -5095,7 +5095,7 @@
         <v>43.7253836039355</v>
       </c>
       <c r="E181">
-        <v>1.56239827290284</v>
+        <v>1.542650938965088</v>
       </c>
       <c r="F181">
         <v>1</v>
@@ -5121,7 +5121,7 @@
         <v>42.04901149545215</v>
       </c>
       <c r="E182">
-        <v>1.646046691760098</v>
+        <v>1.613773772169609</v>
       </c>
       <c r="F182">
         <v>1</v>
@@ -5147,7 +5147,7 @@
         <v>38.14513124281971</v>
       </c>
       <c r="E183">
-        <v>1.562638163916179</v>
+        <v>1.516554602134272</v>
       </c>
       <c r="F183">
         <v>1</v>
@@ -5173,7 +5173,7 @@
         <v>36.44579513285029</v>
       </c>
       <c r="E184">
-        <v>1.486198847372713</v>
+        <v>1.43991228614428</v>
       </c>
       <c r="F184">
         <v>1</v>
@@ -5199,7 +5199,7 @@
         <v>34.76942302436694</v>
       </c>
       <c r="E185">
-        <v>1.660193069553026</v>
+        <v>1.61182286190844</v>
       </c>
       <c r="F185">
         <v>1</v>
@@ -5225,7 +5225,7 @@
         <v>33.41454693668862</v>
       </c>
       <c r="E186">
-        <v>1.800818536794649</v>
+        <v>1.750764286156185</v>
       </c>
       <c r="F186">
         <v>1</v>
@@ -5251,7 +5251,7 @@
         <v>33.57529494709114</v>
       </c>
       <c r="E187">
-        <v>1.784134159325304</v>
+        <v>1.734279710397978</v>
       </c>
       <c r="F187">
         <v>1</v>
@@ -5277,7 +5277,7 @@
         <v>34.24125099018726</v>
       </c>
       <c r="E188">
-        <v>1.715013166952303</v>
+        <v>1.66598646797112</v>
       </c>
       <c r="F188">
         <v>1</v>
@@ -5303,7 +5303,7 @@
         <v>34.99906303922768</v>
       </c>
       <c r="E189">
-        <v>1.636358244596819</v>
+        <v>1.588273467968144</v>
       </c>
       <c r="F189">
         <v>1</v>
@@ -5329,7 +5329,7 @@
         <v>35.68798308380987</v>
       </c>
       <c r="E190">
-        <v>1.564853769728197</v>
+        <v>1.517625286147256</v>
       </c>
       <c r="F190">
         <v>1</v>
@@ -5355,7 +5355,7 @@
         <v>45.44768371539099</v>
       </c>
       <c r="E191">
-        <v>1.476458116542644</v>
+        <v>1.469579534987839</v>
       </c>
       <c r="F191">
         <v>1</v>
@@ -5381,7 +5381,7 @@
         <v>45.44768371539099</v>
       </c>
       <c r="E192">
-        <v>1.476458116542644</v>
+        <v>1.469579534987839</v>
       </c>
       <c r="F192">
         <v>1</v>
@@ -5407,7 +5407,7 @@
         <v>43.33499557867225</v>
       </c>
       <c r="E193">
-        <v>1.581878041677818</v>
+        <v>1.559213790533264</v>
       </c>
       <c r="F193">
         <v>1</v>
@@ -5433,7 +5433,7 @@
         <v>41.33712744938389</v>
       </c>
       <c r="E194">
-        <v>1.681568623055645</v>
+        <v>1.643976619146871</v>
       </c>
       <c r="F194">
         <v>1</v>
@@ -5459,7 +5459,7 @@
         <v>39.08665530374871</v>
       </c>
       <c r="E195">
-        <v>1.646766221420209</v>
+        <v>1.600479649734768</v>
       </c>
       <c r="F195">
         <v>1</v>
@@ -5485,7 +5485,7 @@
         <v>37.57103120566787</v>
       </c>
       <c r="E196">
-        <v>1.511340567877136</v>
+        <v>1.465380792621774</v>
       </c>
       <c r="F196">
         <v>1</v>
@@ -5511,7 +5511,7 @@
         <v>35.55019907489343</v>
       </c>
       <c r="E197">
-        <v>1.579154664701921</v>
+        <v>1.531754922511434</v>
       </c>
       <c r="F197">
         <v>1</v>
@@ -5537,7 +5537,7 @@
         <v>34.31014299464548</v>
       </c>
       <c r="E198">
-        <v>1.707862719465441</v>
+        <v>1.658921649789031</v>
       </c>
       <c r="F198">
         <v>1</v>
@@ -5563,7 +5563,7 @@
         <v>34.33310699613155</v>
       </c>
       <c r="E199">
-        <v>1.70547923696982</v>
+        <v>1.656566710395002</v>
       </c>
       <c r="F199">
         <v>1</v>
@@ -5589,7 +5589,7 @@
         <v>35.73391108678202</v>
       </c>
       <c r="E200">
-        <v>1.560086804736956</v>
+        <v>1.512915407359197</v>
       </c>
       <c r="F200">
         <v>1</v>
@@ -5615,7 +5615,7 @@
         <v>36.76729115365531</v>
       </c>
       <c r="E201">
-        <v>1.452830092434023</v>
+        <v>1.406943134627866</v>
       </c>
       <c r="F201">
         <v>1</v>
@@ -5641,7 +5641,7 @@
         <v>45.88399974362638</v>
       </c>
       <c r="E202">
-        <v>1.446053877613458</v>
+        <v>1.441662885158715</v>
       </c>
       <c r="F202">
         <v>1</v>
@@ -5667,7 +5667,7 @@
         <v>44.5750516589202</v>
       </c>
       <c r="E203">
-        <v>1.520001129098477</v>
+        <v>1.506602379669645</v>
       </c>
       <c r="F203">
         <v>1</v>
@@ -5693,7 +5693,7 @@
         <v>42.53125552665969</v>
       </c>
       <c r="E204">
-        <v>1.621983447979243</v>
+        <v>1.593313779055979</v>
       </c>
       <c r="F204">
         <v>1</v>
@@ -5719,7 +5719,7 @@
         <v>41.22230744195352</v>
       </c>
       <c r="E205">
-        <v>1.687297966812992</v>
+        <v>1.648848046078688</v>
       </c>
       <c r="F205">
         <v>1</v>
@@ -5745,7 +5745,7 @@
         <v>39.24740331415121</v>
       </c>
       <c r="E206">
-        <v>1.661129548311141</v>
+        <v>1.614808316398267</v>
       </c>
       <c r="F206">
         <v>1</v>
@@ -5771,7 +5771,7 @@
         <v>38.12216724133363</v>
       </c>
       <c r="E207">
-        <v>1.560586260074617</v>
+        <v>1.514507649753772</v>
       </c>
       <c r="F207">
         <v>1</v>
@@ -5797,7 +5797,7 @@
         <v>36.90507516257176</v>
       </c>
       <c r="E208">
-        <v>1.451835356471846</v>
+        <v>1.406019173587277</v>
       </c>
       <c r="F208">
         <v>1</v>
@@ -5823,7 +5823,7 @@
         <v>35.38945106449092</v>
       </c>
       <c r="E209">
-        <v>1.595839042171267</v>
+        <v>1.548239498269641</v>
       </c>
       <c r="F209">
         <v>1</v>
@@ -5849,7 +5849,7 @@
         <v>35.38945106449092</v>
       </c>
       <c r="E210">
-        <v>1.595839042171267</v>
+        <v>1.548239498269641</v>
       </c>
       <c r="F210">
         <v>1</v>
@@ -5875,7 +5875,7 @@
         <v>36.9510031655439</v>
       </c>
       <c r="E211">
-        <v>1.455939164154969</v>
+        <v>1.410113078348277</v>
       </c>
       <c r="F211">
         <v>1</v>
@@ -5901,7 +5901,7 @@
         <v>38.5814472710551</v>
       </c>
       <c r="E212">
-        <v>1.601624336905851</v>
+        <v>1.55544669736377</v>
       </c>
       <c r="F212">
         <v>1</v>
@@ -5927,7 +5927,7 @@
         <v>45.67732373025171</v>
       </c>
       <c r="E213">
-        <v>1.464999429027951</v>
+        <v>1.459836681124206</v>
       </c>
       <c r="F213">
         <v>1</v>
@@ -5953,7 +5953,7 @@
         <v>45.76917973619601</v>
       </c>
       <c r="E214">
-        <v>1.460415954022074</v>
+        <v>1.455939539578753</v>
       </c>
       <c r="F214">
         <v>1</v>
@@ -5979,7 +5979,7 @@
         <v>44.46023165148983</v>
       </c>
       <c r="E215">
-        <v>1.525730472855823</v>
+        <v>1.511473806601461</v>
       </c>
       <c r="F215">
         <v>1</v>
@@ -6005,7 +6005,7 @@
         <v>42.3475435147711</v>
       </c>
       <c r="E216">
-        <v>1.631150397990997</v>
+        <v>1.601108062146886</v>
       </c>
       <c r="F216">
         <v>1</v>
@@ -6031,7 +6031,7 @@
         <v>41.19934344046744</v>
       </c>
       <c r="E217">
-        <v>1.688443835564461</v>
+        <v>1.649822331465051</v>
       </c>
       <c r="F217">
         <v>1</v>
@@ -6057,7 +6057,7 @@
         <v>39.54593533347017</v>
       </c>
       <c r="E218">
-        <v>1.687804298251444</v>
+        <v>1.641418697344766</v>
       </c>
       <c r="F218">
         <v>1</v>
@@ -6083,7 +6083,7 @@
         <v>38.55848326956902</v>
       </c>
       <c r="E219">
-        <v>1.59957243306429</v>
+        <v>1.55339974498327</v>
       </c>
       <c r="F219">
         <v>1</v>
@@ -6109,7 +6109,7 @@
         <v>36.92803916405782</v>
       </c>
       <c r="E220">
-        <v>1.453887260313408</v>
+        <v>1.408066125967777</v>
       </c>
       <c r="F220">
         <v>1</v>
@@ -6135,7 +6135,7 @@
         <v>36.33097512541992</v>
       </c>
       <c r="E221">
-        <v>1.498116259850817</v>
+        <v>1.451686983114428</v>
       </c>
       <c r="F221">
         <v>1</v>
@@ -6161,7 +6161,7 @@
         <v>36.65247114622495</v>
       </c>
       <c r="E222">
-        <v>1.464747504912127</v>
+        <v>1.418717831598014</v>
       </c>
       <c r="F222">
         <v>1</v>
@@ -6187,7 +6187,7 @@
         <v>38.76515928294369</v>
       </c>
       <c r="E223">
-        <v>1.618039567638345</v>
+        <v>1.571822316407769</v>
       </c>
       <c r="F223">
         <v>1</v>
@@ -6213,7 +6213,7 @@
         <v>40.00521536319164</v>
       </c>
       <c r="E224">
-        <v>1.728842375082678</v>
+        <v>1.682357744954764</v>
       </c>
       <c r="F224">
         <v>1</v>
@@ -6239,7 +6239,7 @@
         <v>45.33286370796063</v>
       </c>
       <c r="E225">
-        <v>1.48218746029999</v>
+        <v>1.474450961919656</v>
       </c>
       <c r="F225">
         <v>1</v>
@@ -6265,7 +6265,7 @@
         <v>46.48106378226429</v>
       </c>
       <c r="E226">
-        <v>1.191810241142256</v>
+        <v>1.171795550419505</v>
       </c>
       <c r="F226">
         <v>1</v>
@@ -6291,7 +6291,7 @@
         <v>45.65435972876564</v>
       </c>
       <c r="E227">
-        <v>1.46614529777942</v>
+        <v>1.46081096651057</v>
       </c>
       <c r="F227">
         <v>1</v>
@@ -6317,7 +6317,7 @@
         <v>44.34541164405947</v>
       </c>
       <c r="E228">
-        <v>1.531459816613169</v>
+        <v>1.516345233533278</v>
       </c>
       <c r="F228">
         <v>1</v>
@@ -6343,7 +6343,7 @@
         <v>42.27865151031288</v>
       </c>
       <c r="E229">
-        <v>1.634588004245405</v>
+        <v>1.604030918305976</v>
       </c>
       <c r="F229">
         <v>1</v>
@@ -6369,7 +6369,7 @@
         <v>41.63565946870284</v>
       </c>
       <c r="E230">
-        <v>1.666672329286545</v>
+        <v>1.631310909124148</v>
       </c>
       <c r="F230">
         <v>1</v>
@@ -6395,7 +6395,7 @@
         <v>39.56889933495624</v>
       </c>
       <c r="E231">
-        <v>1.689856202093005</v>
+        <v>1.643465649725266</v>
       </c>
       <c r="F231">
         <v>1</v>
@@ -6421,7 +6421,7 @@
         <v>38.65033927551332</v>
       </c>
       <c r="E232">
-        <v>1.607780048430536</v>
+        <v>1.56158755450527</v>
       </c>
       <c r="F232">
         <v>1</v>
@@ -6447,7 +6447,7 @@
         <v>37.04285917148819</v>
       </c>
       <c r="E233">
-        <v>1.464146779521216</v>
+        <v>1.418300887870277</v>
       </c>
       <c r="F233">
         <v>1</v>
@@ -6473,7 +6473,7 @@
         <v>37.08878717446034</v>
       </c>
       <c r="E234">
-        <v>1.46825058720434</v>
+        <v>1.422394792631277</v>
       </c>
       <c r="F234">
         <v>1</v>
@@ -6499,7 +6499,7 @@
         <v>37.70881521458431</v>
       </c>
       <c r="E235">
-        <v>1.523651990926506</v>
+        <v>1.477662506904774</v>
       </c>
       <c r="F235">
         <v>1</v>
@@ -6525,7 +6525,7 @@
         <v>39.24740331415121</v>
       </c>
       <c r="E236">
-        <v>1.661129548311141</v>
+        <v>1.614808316398267</v>
       </c>
       <c r="F236">
         <v>1</v>
@@ -6551,7 +6551,7 @@
         <v>40.23485537805237</v>
       </c>
       <c r="E237">
-        <v>1.736570323126171</v>
+        <v>1.69074231769231</v>
       </c>
       <c r="F237">
         <v>1</v>
@@ -6577,7 +6577,7 @@
         <v>46.66477579415287</v>
       </c>
       <c r="E238">
-        <v>1.196410853685324</v>
+        <v>1.176152820792267</v>
       </c>
       <c r="F238">
         <v>1</v>
@@ -6603,7 +6603,7 @@
         <v>46.6418117926668</v>
       </c>
       <c r="E239">
-        <v>1.19583577711744</v>
+        <v>1.175608161995672</v>
       </c>
       <c r="F239">
         <v>1</v>
@@ -6629,7 +6629,7 @@
         <v>48.01965188183119</v>
       </c>
       <c r="E240">
-        <v>1.23034037119045</v>
+        <v>1.208287689791385</v>
       </c>
       <c r="F240">
         <v>1</v>
@@ -6655,7 +6655,7 @@
         <v>47.65222785805402</v>
       </c>
       <c r="E241">
-        <v>1.221139146104314</v>
+        <v>1.199573149045861</v>
       </c>
       <c r="F241">
         <v>1</v>
@@ -6681,7 +6681,7 @@
         <v>45.90696374511245</v>
       </c>
       <c r="E242">
-        <v>1.43627527621072</v>
+        <v>1.43128337228413</v>
       </c>
       <c r="F242">
         <v>1</v>
@@ -6707,7 +6707,7 @@
         <v>44.71283566783664</v>
       </c>
       <c r="E243">
-        <v>1.513125916589661</v>
+        <v>1.500756667351465</v>
       </c>
       <c r="F243">
         <v>1</v>
@@ -6733,7 +6733,7 @@
         <v>42.41643551922932</v>
       </c>
       <c r="E244">
-        <v>1.627712791736589</v>
+        <v>1.598185205987796</v>
       </c>
       <c r="F244">
         <v>1</v>
@@ -6759,7 +6759,7 @@
         <v>42.0949394984243</v>
       </c>
       <c r="E245">
-        <v>1.643754954257159</v>
+        <v>1.611825201396882</v>
       </c>
       <c r="F245">
         <v>1</v>
@@ -6785,7 +6785,7 @@
         <v>39.56889933495624</v>
       </c>
       <c r="E246">
-        <v>1.689856202093005</v>
+        <v>1.643465649725266</v>
       </c>
       <c r="F246">
         <v>1</v>
@@ -6811,7 +6811,7 @@
         <v>38.62737527402724</v>
       </c>
       <c r="E247">
-        <v>1.605728144588975</v>
+        <v>1.55954060212477</v>
       </c>
       <c r="F247">
         <v>1</v>
@@ -6837,7 +6837,7 @@
         <v>38.25995125025007</v>
       </c>
       <c r="E248">
-        <v>1.572897683123987</v>
+        <v>1.526789364036772</v>
       </c>
       <c r="F248">
         <v>1</v>
@@ -6863,7 +6863,7 @@
         <v>38.92590729334619</v>
       </c>
       <c r="E249">
-        <v>1.632402894529277</v>
+        <v>1.586150983071269</v>
       </c>
       <c r="F249">
         <v>1</v>
@@ -6889,7 +6889,7 @@
         <v>39.24740331415121</v>
       </c>
       <c r="E250">
-        <v>1.661129548311141</v>
+        <v>1.614808316398267</v>
       </c>
       <c r="F250">
         <v>1</v>
@@ -6915,7 +6915,7 @@
         <v>40.39560338845489</v>
       </c>
       <c r="E251">
-        <v>1.728549241865886</v>
+        <v>1.683922319987767</v>
       </c>
       <c r="F251">
         <v>1</v>
@@ -6941,7 +6941,7 @@
         <v>48.4330039085805</v>
       </c>
       <c r="E252">
-        <v>1.240691749412353</v>
+        <v>1.218091548130099</v>
       </c>
       <c r="F252">
         <v>1</v>
@@ -6967,7 +6967,7 @@
         <v>48.82339193384375</v>
       </c>
       <c r="E253">
-        <v>1.250468051066373</v>
+        <v>1.227350747672218</v>
       </c>
       <c r="F253">
         <v>1</v>
@@ -6993,7 +6993,7 @@
         <v>48.47893191155265</v>
       </c>
       <c r="E254">
-        <v>1.24184190254812</v>
+        <v>1.21918086572329</v>
       </c>
       <c r="F254">
         <v>1</v>
@@ -7019,7 +7019,7 @@
         <v>46.73366779861109</v>
       </c>
       <c r="E255">
-        <v>1.198136083388974</v>
+        <v>1.177786797182053</v>
       </c>
       <c r="F255">
         <v>1</v>
@@ -7045,7 +7045,7 @@
         <v>45.56250372282135</v>
       </c>
       <c r="E256">
-        <v>1.470728772785298</v>
+        <v>1.464708108056023</v>
       </c>
       <c r="F256">
         <v>1</v>
@@ -7071,7 +7071,7 @@
         <v>43.95502361879623</v>
       </c>
       <c r="E257">
-        <v>1.550939585388147</v>
+        <v>1.532908085101454</v>
       </c>
       <c r="F257">
         <v>1</v>
@@ -7097,7 +7097,7 @@
         <v>42.53125552665969</v>
       </c>
       <c r="E258">
-        <v>1.621983447979243</v>
+        <v>1.593313779055979</v>
       </c>
       <c r="F258">
         <v>1</v>
@@ -7123,7 +7123,7 @@
         <v>41.4978754597864</v>
       </c>
       <c r="E259">
-        <v>1.67354754179536</v>
+        <v>1.637156621442328</v>
       </c>
       <c r="F259">
         <v>1</v>
@@ -7149,7 +7149,7 @@
         <v>40.44153139142702</v>
       </c>
       <c r="E260">
-        <v>1.726257504362948</v>
+        <v>1.681973749215041</v>
       </c>
       <c r="F260">
         <v>1</v>
@@ -7175,7 +7175,7 @@
         <v>39.63779133941446</v>
       </c>
       <c r="E261">
-        <v>1.69601191361769</v>
+        <v>1.649606506866766</v>
       </c>
       <c r="F261">
         <v>1</v>
@@ -7201,7 +7201,7 @@
         <v>39.82150335130305</v>
       </c>
       <c r="E262">
-        <v>1.712427144350184</v>
+        <v>1.665982125910765</v>
       </c>
       <c r="F262">
         <v>1</v>
@@ -7227,7 +7227,7 @@
         <v>40.46449539291309</v>
       </c>
       <c r="E263">
-        <v>1.725111635611478</v>
+        <v>1.680999463828677</v>
       </c>
       <c r="F263">
         <v>1</v>
@@ -7253,7 +7253,7 @@
         <v>41.24527144343959</v>
       </c>
       <c r="E264">
-        <v>1.686152098061523</v>
+        <v>1.647873760692325</v>
       </c>
       <c r="F264">
         <v>1</v>
@@ -7279,7 +7279,7 @@
         <v>49.76491599477275</v>
       </c>
       <c r="E265">
-        <v>1.274046190349597</v>
+        <v>1.249681758332622</v>
       </c>
       <c r="F265">
         <v>1</v>
@@ -7305,7 +7305,7 @@
         <v>49.90270000368919</v>
       </c>
       <c r="E266">
-        <v>1.277496649756898</v>
+        <v>1.252949711112194</v>
       </c>
       <c r="F266">
         <v>1</v>
@@ -7331,7 +7331,7 @@
         <v>49.213779959107</v>
       </c>
       <c r="E267">
-        <v>1.260244352720393</v>
+        <v>1.236609947214337</v>
       </c>
       <c r="F267">
         <v>1</v>
@@ -7357,7 +7357,7 @@
         <v>47.97372387885905</v>
       </c>
       <c r="E268">
-        <v>1.229190218054683</v>
+        <v>1.207198372198195</v>
       </c>
       <c r="F268">
         <v>1</v>
@@ -7383,7 +7383,7 @@
         <v>46.77959580158323</v>
       </c>
       <c r="E269">
-        <v>1.199286236524741</v>
+        <v>1.178876114775243</v>
       </c>
       <c r="F269">
         <v>1</v>
@@ -7409,7 +7409,7 @@
         <v>45.44768371539099</v>
       </c>
       <c r="E270">
-        <v>1.476458116542644</v>
+        <v>1.469579534987839</v>
       </c>
       <c r="F270">
         <v>1</v>
@@ -7435,7 +7435,7 @@
         <v>44.39133964703161</v>
       </c>
       <c r="E271">
-        <v>1.529168079110231</v>
+        <v>1.514396662760551</v>
       </c>
       <c r="F271">
         <v>1</v>
@@ -7461,7 +7461,7 @@
         <v>43.10535556381151</v>
       </c>
       <c r="E272">
-        <v>1.593336729192511</v>
+        <v>1.568956644396897</v>
       </c>
       <c r="F272">
         <v>1</v>
@@ -7487,7 +7487,7 @@
         <v>42.18679550436859</v>
       </c>
       <c r="E273">
-        <v>1.639171479251282</v>
+        <v>1.607928059851429</v>
       </c>
       <c r="F273">
         <v>1</v>
@@ -7513,7 +7513,7 @@
         <v>41.17637943898137</v>
       </c>
       <c r="E274">
-        <v>1.68958970431593</v>
+        <v>1.650796616851415</v>
       </c>
       <c r="F274">
         <v>1</v>
@@ -7539,7 +7539,7 @@
         <v>41.52083946127247</v>
       </c>
       <c r="E275">
-        <v>1.672401673043891</v>
+        <v>1.636182336055965</v>
       </c>
       <c r="F275">
         <v>1</v>
@@ -7565,7 +7565,7 @@
         <v>42.20975950585466</v>
       </c>
       <c r="E276">
-        <v>1.638025610499813</v>
+        <v>1.606953774465066</v>
       </c>
       <c r="F276">
         <v>1</v>
@@ -7591,7 +7591,7 @@
         <v>42.69200353706221</v>
       </c>
       <c r="E277">
-        <v>1.613962366718958</v>
+        <v>1.586493781351436</v>
       </c>
       <c r="F277">
         <v>1</v>
@@ -7617,7 +7617,7 @@
         <v>44.02391562325445</v>
       </c>
       <c r="E278">
-        <v>1.547501979133739</v>
+        <v>1.529985228942364</v>
       </c>
       <c r="F278">
         <v>1</v>
@@ -7643,7 +7643,7 @@
         <v>51.30350409433966</v>
       </c>
       <c r="E279">
-        <v>1.312576320397791</v>
+        <v>1.286173897704503</v>
       </c>
       <c r="F279">
         <v>1</v>
@@ -7669,7 +7669,7 @@
         <v>50.86718806610426</v>
       </c>
       <c r="E280">
-        <v>1.301649865608005</v>
+        <v>1.275825380569193</v>
       </c>
       <c r="F280">
         <v>1</v>
@@ -7695,7 +7695,7 @@
         <v>49.8108439977449</v>
       </c>
       <c r="E281">
-        <v>1.275196343485364</v>
+        <v>1.250771075925813</v>
       </c>
       <c r="F281">
         <v>1</v>
@@ -7721,7 +7721,7 @@
         <v>49.05303194870449</v>
       </c>
       <c r="E282">
-        <v>1.256218816745208</v>
+        <v>1.23279733563817</v>
       </c>
       <c r="F282">
         <v>1</v>
@@ -7747,7 +7747,7 @@
         <v>47.4914798476515</v>
       </c>
       <c r="E283">
-        <v>1.21711361012913</v>
+        <v>1.195760537469695</v>
       </c>
       <c r="F283">
         <v>1</v>
@@ -7773,7 +7773,7 @@
         <v>46.36624377483392</v>
       </c>
       <c r="E284">
-        <v>1.240703248155948</v>
+        <v>1.22369311479243</v>
       </c>
       <c r="F284">
         <v>1</v>
@@ -7799,7 +7799,7 @@
         <v>45.30989970647455</v>
       </c>
       <c r="E285">
-        <v>1.48333332905146</v>
+        <v>1.475425247306019</v>
       </c>
       <c r="F285">
         <v>1</v>
@@ -7825,7 +7825,7 @@
         <v>43.74834760542157</v>
       </c>
       <c r="E286">
-        <v>1.561252404151371</v>
+        <v>1.541676653578724</v>
       </c>
       <c r="F286">
         <v>1</v>
@@ -7851,7 +7851,7 @@
         <v>42.73793154003435</v>
       </c>
       <c r="E287">
-        <v>1.611670629216019</v>
+        <v>1.58454521057871</v>
       </c>
       <c r="F287">
         <v>1</v>
@@ -7877,7 +7877,7 @@
         <v>42.69200353706221</v>
       </c>
       <c r="E288">
-        <v>1.613962366718958</v>
+        <v>1.586493781351436</v>
       </c>
       <c r="F288">
         <v>1</v>
@@ -7903,7 +7903,7 @@
         <v>43.35795958015832</v>
       </c>
       <c r="E289">
-        <v>1.580732172926349</v>
+        <v>1.5582395051469</v>
       </c>
       <c r="F289">
         <v>1</v>
@@ -7929,7 +7929,7 @@
         <v>43.93205961731016</v>
       </c>
       <c r="E290">
-        <v>1.552085454139617</v>
+        <v>1.533882370487818</v>
       </c>
       <c r="F290">
         <v>1</v>
@@ -7955,7 +7955,7 @@
         <v>44.71283566783664</v>
       </c>
       <c r="E291">
-        <v>1.513125916589661</v>
+        <v>1.500756667351465</v>
       </c>
       <c r="F291">
         <v>1</v>
@@ -7981,7 +7981,7 @@
         <v>52.52059617310154</v>
       </c>
       <c r="E292">
-        <v>1.343055378495617</v>
+        <v>1.315040813924049</v>
       </c>
       <c r="F292">
         <v>1</v>
@@ -8007,7 +8007,7 @@
         <v>52.33688416121295</v>
       </c>
       <c r="E293">
-        <v>1.338454765952549</v>
+        <v>1.310683543551288</v>
       </c>
       <c r="F293">
         <v>1</v>
@@ -8033,7 +8033,7 @@
         <v>51.16572008542322</v>
       </c>
       <c r="E294">
-        <v>1.30912586099049</v>
+        <v>1.282905944924931</v>
       </c>
       <c r="F294">
         <v>1</v>
@@ -8059,7 +8059,7 @@
         <v>49.30563596505129</v>
       </c>
       <c r="E295">
-        <v>1.262544658991926</v>
+        <v>1.238788582400718</v>
       </c>
       <c r="F295">
         <v>1</v>
@@ -8085,7 +8085,7 @@
         <v>48.29521989966406</v>
       </c>
       <c r="E296">
-        <v>1.237241290005052</v>
+        <v>1.214823595350528</v>
       </c>
       <c r="F296">
         <v>1</v>
@@ -8111,7 +8111,7 @@
         <v>47.05516381941611</v>
       </c>
       <c r="E297">
-        <v>1.206187155339343</v>
+        <v>1.185412020334386</v>
       </c>
       <c r="F297">
         <v>1</v>
@@ -8137,7 +8137,7 @@
         <v>45.5165757198492</v>
       </c>
       <c r="E298">
-        <v>1.473020510288236</v>
+        <v>1.466656678828749</v>
       </c>
       <c r="F298">
         <v>1</v>
@@ -8163,7 +8163,7 @@
         <v>44.16169963217089</v>
       </c>
       <c r="E299">
-        <v>1.540626766624924</v>
+        <v>1.524139516624185</v>
       </c>
       <c r="F299">
         <v>1</v>
@@ -8189,7 +8189,7 @@
         <v>43.77131160690764</v>
       </c>
       <c r="E300">
-        <v>1.560106535399902</v>
+        <v>1.540702368192361</v>
       </c>
       <c r="F300">
         <v>1</v>
@@ -8215,7 +8215,7 @@
         <v>45.0113676871556</v>
       </c>
       <c r="E301">
-        <v>1.49822962282056</v>
+        <v>1.488090957328742</v>
       </c>
       <c r="F301">
         <v>1</v>
@@ -8241,7 +8241,7 @@
         <v>45.56250372282135</v>
       </c>
       <c r="E302">
-        <v>1.470728772785298</v>
+        <v>1.464708108056023</v>
       </c>
       <c r="F302">
         <v>1</v>
@@ -8267,7 +8267,7 @@
         <v>45.70028773173779</v>
       </c>
       <c r="E303">
-        <v>1.463853560276482</v>
+        <v>1.458862395737843</v>
       </c>
       <c r="F303">
         <v>1</v>
@@ -8293,7 +8293,7 @@
         <v>46.50402778375036</v>
       </c>
       <c r="E304">
-        <v>1.192385317710139</v>
+        <v>1.1723402092161</v>
       </c>
       <c r="F304">
         <v>1</v>
@@ -8319,7 +8319,7 @@
         <v>53.89843626226593</v>
       </c>
       <c r="E305">
-        <v>1.377559972568627</v>
+        <v>1.347720341719763</v>
       </c>
       <c r="F305">
         <v>1</v>
@@ -8345,7 +8345,7 @@
         <v>53.6687962474052</v>
       </c>
       <c r="E306">
-        <v>1.371809206889792</v>
+        <v>1.342273753753811</v>
       </c>
       <c r="F306">
         <v>1</v>
@@ -8371,7 +8371,7 @@
         <v>52.88802019687871</v>
       </c>
       <c r="E307">
-        <v>1.352256603581753</v>
+        <v>1.323755354669573</v>
       </c>
       <c r="F307">
         <v>1</v>
@@ -8397,7 +8397,7 @@
         <v>50.22419602449422</v>
       </c>
       <c r="E308">
-        <v>1.285547721707267</v>
+        <v>1.260574934264527</v>
       </c>
       <c r="F308">
         <v>1</v>
@@ -8423,7 +8423,7 @@
         <v>48.38707590560836</v>
       </c>
       <c r="E309">
-        <v>1.239541596276586</v>
+        <v>1.217002230536909</v>
       </c>
       <c r="F309">
         <v>1</v>
@@ -8449,7 +8449,7 @@
         <v>47.46851584616543</v>
       </c>
       <c r="E310">
-        <v>1.216538533561246</v>
+        <v>1.1952158786731</v>
       </c>
       <c r="F310">
         <v>1</v>
@@ -8475,7 +8475,7 @@
         <v>46.15956776145926</v>
       </c>
       <c r="E311">
-        <v>1.328710660780596</v>
+        <v>1.317108730663695</v>
       </c>
       <c r="F311">
         <v>1</v>
@@ -8501,7 +8501,7 @@
         <v>45.05729569012775</v>
       </c>
       <c r="E312">
-        <v>1.495937885317622</v>
+        <v>1.486142386556015</v>
       </c>
       <c r="F312">
         <v>1</v>
@@ -8527,7 +8527,7 @@
         <v>45.47064771687707</v>
       </c>
       <c r="E313">
-        <v>1.475312247791175</v>
+        <v>1.468605249601476</v>
       </c>
       <c r="F313">
         <v>1</v>
@@ -8553,7 +8553,7 @@
         <v>46.54995578672251</v>
       </c>
       <c r="E314">
-        <v>1.193535470845906</v>
+        <v>1.173429526809291</v>
       </c>
       <c r="F314">
         <v>1</v>
@@ -8579,7 +8579,7 @@
         <v>47.9277958758869</v>
       </c>
       <c r="E315">
-        <v>1.228040064918916</v>
+        <v>1.206109054605004</v>
       </c>
       <c r="F315">
         <v>1</v>
@@ -8605,7 +8605,7 @@
         <v>48.11150788777547</v>
       </c>
       <c r="E316">
-        <v>1.232640677461984</v>
+        <v>1.210466324977766</v>
       </c>
       <c r="F316">
         <v>1</v>
@@ -8631,7 +8631,7 @@
         <v>55.09256433954174</v>
       </c>
       <c r="E317">
-        <v>1.40746395409857</v>
+        <v>1.376042599142715</v>
       </c>
       <c r="F317">
         <v>1</v>
@@ -8657,7 +8657,7 @@
         <v>54.17400428009881</v>
       </c>
       <c r="E318">
-        <v>1.384460891383229</v>
+        <v>1.354256247278906</v>
       </c>
       <c r="F318">
         <v>1</v>
@@ -8683,7 +8683,7 @@
         <v>52.97987620282301</v>
       </c>
       <c r="E319">
-        <v>1.354556909853287</v>
+        <v>1.325933989855954</v>
       </c>
       <c r="F319">
         <v>1</v>
@@ -8709,7 +8709,7 @@
         <v>51.32646809582573</v>
       </c>
       <c r="E320">
-        <v>1.313151396965675</v>
+        <v>1.286718556501098</v>
       </c>
       <c r="F320">
         <v>1</v>
@@ -8735,7 +8735,7 @@
         <v>49.76491599477275</v>
       </c>
       <c r="E321">
-        <v>1.274046190349597</v>
+        <v>1.249681758332622</v>
       </c>
       <c r="F321">
         <v>1</v>
@@ -8761,7 +8761,7 @@
         <v>48.13447188926155</v>
       </c>
       <c r="E322">
-        <v>1.233215754029868</v>
+        <v>1.211010983774361</v>
       </c>
       <c r="F322">
         <v>1</v>
@@ -8787,7 +8787,7 @@
         <v>47.2388758313047</v>
       </c>
       <c r="E323">
-        <v>1.210787767882411</v>
+        <v>1.189769290707148</v>
       </c>
       <c r="F323">
         <v>1</v>
@@ -8813,7 +8813,7 @@
         <v>46.27438776888962</v>
       </c>
       <c r="E324">
-        <v>1.279817653766903</v>
+        <v>1.26521116629077</v>
       </c>
       <c r="F324">
         <v>1</v>
@@ -8839,7 +8839,7 @@
         <v>46.73366779861109</v>
       </c>
       <c r="E325">
-        <v>1.198136083388974</v>
+        <v>1.177786797182053</v>
       </c>
       <c r="F325">
         <v>1</v>
@@ -8865,7 +8865,7 @@
         <v>48.66264392344124</v>
       </c>
       <c r="E326">
-        <v>1.246442515091188</v>
+        <v>1.223538136096052</v>
       </c>
       <c r="F326">
         <v>1</v>
@@ -8891,7 +8891,7 @@
         <v>56.42447642573399</v>
       </c>
       <c r="E327">
-        <v>1.440818395035813</v>
+        <v>1.407632809345238</v>
       </c>
       <c r="F327">
         <v>1</v>
@@ -8917,7 +8917,7 @@
         <v>55.59777237223535</v>
       </c>
       <c r="E328">
-        <v>1.420115638592007</v>
+        <v>1.38802509266781</v>
       </c>
       <c r="F328">
         <v>1</v>
@@ -8943,7 +8943,7 @@
         <v>54.5184643023899</v>
       </c>
       <c r="E329">
-        <v>1.393087039901482</v>
+        <v>1.362426129227834</v>
       </c>
       <c r="F329">
         <v>1</v>
@@ -8969,7 +8969,7 @@
         <v>52.58948817755976</v>
       </c>
       <c r="E330">
-        <v>1.344780608199268</v>
+        <v>1.316674790313835</v>
       </c>
       <c r="F330">
         <v>1</v>
@@ -8995,7 +8995,7 @@
         <v>51.16572008542322</v>
       </c>
       <c r="E331">
-        <v>1.30912586099049</v>
+        <v>1.282905944924931</v>
       </c>
       <c r="F331">
         <v>1</v>
@@ -9021,7 +9021,7 @@
         <v>49.44341997396772</v>
       </c>
       <c r="E332">
-        <v>1.265995118399228</v>
+        <v>1.242056535180289</v>
       </c>
       <c r="F332">
         <v>1</v>
@@ -9047,7 +9047,7 @@
         <v>48.96117594276019</v>
       </c>
       <c r="E333">
-        <v>1.253918510473674</v>
+        <v>1.230618700451789</v>
       </c>
       <c r="F333">
         <v>1</v>
@@ -9073,7 +9073,7 @@
         <v>47.99668788034512</v>
       </c>
       <c r="E334">
-        <v>1.229765294622567</v>
+        <v>1.20774303099479</v>
       </c>
       <c r="F334">
         <v>1</v>
@@ -9099,7 +9099,7 @@
         <v>48.06557988480333</v>
       </c>
       <c r="E335">
-        <v>1.231490524326217</v>
+        <v>1.209377007384576</v>
       </c>
       <c r="F335">
         <v>1</v>
@@ -9125,7 +9125,7 @@
         <v>49.83380799923097</v>
       </c>
       <c r="E336">
-        <v>1.275771420053247</v>
+        <v>1.251315734722408</v>
       </c>
       <c r="F336">
         <v>1</v>
@@ -9151,7 +9151,7 @@
         <v>57.68749650746801</v>
       </c>
       <c r="E337">
-        <v>1.472447606269406</v>
+        <v>1.437589043157975</v>
       </c>
       <c r="F337">
         <v>1</v>
@@ -9177,7 +9177,7 @@
         <v>57.66453250598194</v>
       </c>
       <c r="E338">
-        <v>1.471872529701522</v>
+        <v>1.43704438436138</v>
       </c>
       <c r="F338">
         <v>1</v>
@@ -9203,7 +9203,7 @@
         <v>55.2992403529164</v>
       </c>
       <c r="E339">
-        <v>1.412639643209521</v>
+        <v>1.380944528312072</v>
       </c>
       <c r="F339">
         <v>1</v>
@@ -9229,7 +9229,7 @@
         <v>53.59990424294698</v>
       </c>
       <c r="E340">
-        <v>1.370083977186142</v>
+        <v>1.340639777364025</v>
       </c>
       <c r="F340">
         <v>1</v>
@@ -9255,7 +9255,7 @@
         <v>51.99242413892185</v>
       </c>
       <c r="E341">
-        <v>1.329828617434297</v>
+        <v>1.302513661602359</v>
       </c>
       <c r="F341">
         <v>1</v>
@@ -9281,7 +9281,7 @@
         <v>50.93608007056248</v>
       </c>
       <c r="E342">
-        <v>1.303375095311655</v>
+        <v>1.277459356958979</v>
       </c>
       <c r="F342">
         <v>1</v>
@@ -9307,7 +9307,7 @@
         <v>49.99455600963348</v>
       </c>
       <c r="E343">
-        <v>1.279796956028432</v>
+        <v>1.255128346298575</v>
       </c>
       <c r="F343">
         <v>1</v>
@@ -9333,7 +9333,7 @@
         <v>49.25970796207915</v>
       </c>
       <c r="E344">
-        <v>1.26139450585616</v>
+        <v>1.237699264807527</v>
       </c>
       <c r="F344">
         <v>1</v>
@@ -9359,7 +9359,7 @@
         <v>49.30563596505129</v>
       </c>
       <c r="E345">
-        <v>1.262544658991926</v>
+        <v>1.238788582400718</v>
       </c>
       <c r="F345">
         <v>1</v>
@@ -9385,7 +9385,7 @@
         <v>58.69791257285523</v>
       </c>
       <c r="E346">
-        <v>1.49775097525628</v>
+        <v>1.461554030208165</v>
       </c>
       <c r="F346">
         <v>1</v>
@@ -9411,7 +9411,7 @@
         <v>58.12381253570341</v>
       </c>
       <c r="E347">
-        <v>1.483374061059192</v>
+        <v>1.447937560293285</v>
       </c>
       <c r="F347">
         <v>1</v>
@@ -9437,7 +9437,7 @@
         <v>56.53929643316435</v>
       </c>
       <c r="E348">
-        <v>1.44369377787523</v>
+        <v>1.410356103328214</v>
       </c>
       <c r="F348">
         <v>1</v>
@@ -9463,7 +9463,7 @@
         <v>55.11552834102781</v>
       </c>
       <c r="E349">
-        <v>1.408039030666453</v>
+        <v>1.37658725793931</v>
       </c>
       <c r="F349">
         <v>1</v>
@@ -9489,7 +9489,7 @@
         <v>53.04876820728123</v>
       </c>
       <c r="E350">
-        <v>1.356282139556938</v>
+        <v>1.32756796624574</v>
       </c>
       <c r="F350">
         <v>1</v>
@@ -9515,7 +9515,7 @@
         <v>51.90056813297755</v>
       </c>
       <c r="E351">
-        <v>1.327528311162762</v>
+        <v>1.300335026415978</v>
       </c>
       <c r="F351">
         <v>1</v>
@@ -9541,7 +9541,7 @@
         <v>51.05090007799285</v>
       </c>
       <c r="E352">
-        <v>1.306250478151073</v>
+        <v>1.280182650941955</v>
       </c>
       <c r="F352">
         <v>1</v>
@@ -9567,7 +9567,7 @@
         <v>50.56865604678532</v>
       </c>
       <c r="E353">
-        <v>1.294173870225519</v>
+        <v>1.268744816213455</v>
       </c>
       <c r="F353">
         <v>1</v>
@@ -9593,7 +9593,7 @@
         <v>60.0068606575614</v>
       </c>
       <c r="E354">
-        <v>1.53053033962564</v>
+        <v>1.492599581614093</v>
       </c>
       <c r="F354">
         <v>1</v>
@@ -9619,7 +9619,7 @@
         <v>58.65198456988308</v>
       </c>
       <c r="E355">
-        <v>1.496600822120513</v>
+        <v>1.460464712614975</v>
       </c>
       <c r="F355">
         <v>1</v>
@@ -9645,7 +9645,7 @@
         <v>57.25118047923262</v>
       </c>
       <c r="E356">
-        <v>1.461521151479619</v>
+        <v>1.427240526022666</v>
       </c>
       <c r="F356">
         <v>1</v>
@@ -9671,7 +9671,7 @@
         <v>56.12594440641503</v>
       </c>
       <c r="E357">
-        <v>1.433342399653327</v>
+        <v>1.4005522449895</v>
       </c>
       <c r="F357">
         <v>1</v>
@@ -9697,7 +9697,7 @@
         <v>54.0132562696963</v>
       </c>
       <c r="E358">
-        <v>1.380435355408045</v>
+        <v>1.350443635702739</v>
       </c>
       <c r="F358">
         <v>1</v>
@@ -9723,7 +9723,7 @@
         <v>52.56652417607368</v>
       </c>
       <c r="E359">
-        <v>1.344205531631384</v>
+        <v>1.31613013151724</v>
       </c>
       <c r="F359">
         <v>1</v>
@@ -9749,7 +9749,7 @@
         <v>52.26799215675473</v>
       </c>
       <c r="E360">
-        <v>1.336729536248899</v>
+        <v>1.309049567161502</v>
       </c>
       <c r="F360">
         <v>1</v>
@@ -9775,7 +9775,7 @@
         <v>61.01727672294862</v>
       </c>
       <c r="E361">
-        <v>1.555833708612514</v>
+        <v>1.516564568664283</v>
       </c>
       <c r="F361">
         <v>1</v>
@@ -9801,7 +9801,7 @@
         <v>60.19057266944999</v>
       </c>
       <c r="E362">
-        <v>1.535130952168708</v>
+        <v>1.496956851986855</v>
       </c>
       <c r="F362">
         <v>1</v>
@@ -9827,7 +9827,7 @@
         <v>57.73342451044016</v>
       </c>
       <c r="E363">
-        <v>1.473597759405173</v>
+        <v>1.438678360751166</v>
       </c>
       <c r="F363">
         <v>1</v>
@@ -9853,7 +9853,7 @@
         <v>56.79190044951116</v>
       </c>
       <c r="E364">
-        <v>1.450019620121949</v>
+        <v>1.416347350090762</v>
       </c>
       <c r="F364">
         <v>1</v>
@@ -9879,7 +9879,7 @@
         <v>55.16145634399996</v>
       </c>
       <c r="E365">
-        <v>1.40918918380222</v>
+        <v>1.3776765755325</v>
       </c>
       <c r="F365">
         <v>1</v>
@@ -9905,7 +9905,7 @@
         <v>54.44957229793168</v>
       </c>
       <c r="E366">
-        <v>1.391361810197832</v>
+        <v>1.360792152838048</v>
       </c>
       <c r="F366">
         <v>1</v>
@@ -9931,7 +9931,7 @@
         <v>54.56439230536205</v>
       </c>
       <c r="E367">
-        <v>1.394237193037249</v>
+        <v>1.363515446821025</v>
       </c>
       <c r="F367">
         <v>1</v>
@@ -9957,7 +9957,7 @@
         <v>63.29071287006987</v>
       </c>
       <c r="E368">
-        <v>1.612766288832981</v>
+        <v>1.57048578952721</v>
       </c>
       <c r="F368">
         <v>1</v>
@@ -9983,7 +9983,7 @@
         <v>62.14251279576621</v>
       </c>
       <c r="E369">
-        <v>1.584012460438805</v>
+        <v>1.543252849697449</v>
       </c>
       <c r="F369">
         <v>1</v>
@@ -10009,7 +10009,7 @@
         <v>59.52461662635386</v>
       </c>
       <c r="E370">
-        <v>1.518453731700086</v>
+        <v>1.481161746885593</v>
       </c>
       <c r="F370">
         <v>1</v>
@@ -10035,7 +10035,7 @@
         <v>57.73342451044016</v>
       </c>
       <c r="E371">
-        <v>1.473597759405173</v>
+        <v>1.438678360751166</v>
       </c>
       <c r="F371">
         <v>1</v>
@@ -10061,7 +10061,7 @@
         <v>57.06746846734403</v>
       </c>
       <c r="E372">
-        <v>1.456920538936551</v>
+        <v>1.422883255649904</v>
       </c>
       <c r="F372">
         <v>1</v>
@@ -10087,7 +10087,7 @@
         <v>56.86079245396938</v>
       </c>
       <c r="E373">
-        <v>1.451744849825599</v>
+        <v>1.417981326480547</v>
       </c>
       <c r="F373">
         <v>1</v>
@@ -10113,7 +10113,7 @@
         <v>63.33664087304201</v>
       </c>
       <c r="E374">
-        <v>1.613916441968748</v>
+        <v>1.571575107120401</v>
       </c>
       <c r="F374">
         <v>1</v>
@@ -10139,7 +10139,7 @@
         <v>60.92542071700433</v>
       </c>
       <c r="E375">
-        <v>1.55353340234098</v>
+        <v>1.514385933477902</v>
       </c>
       <c r="F375">
         <v>1</v>
@@ -10165,7 +10165,7 @@
         <v>59.43276062040958</v>
       </c>
       <c r="E376">
-        <v>1.516153425428552</v>
+        <v>1.478983111699212</v>
       </c>
       <c r="F376">
         <v>1</v>

</xml_diff>